<commit_message>
Journal de travail SB
</commit_message>
<xml_diff>
--- a/LM_Journal_Travail_V1.0.xlsx
+++ b/LM_Journal_Travail_V1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Love-Mirroring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360E29EA-BD42-4CA0-906F-F7B7B1F1AC71}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9531EC86-20EE-41EE-81D7-02BF88F42C74}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="40">
   <si>
     <t>Jalon</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>Création des User Stories, j'ai identifié par rapport au PBS les différentes Stories du projet et mes collègues passeront le document en revue pour apporter leur point de vue. Nous avons actuellement 15 User Stories à mon premier passage.</t>
+  </si>
+  <si>
+    <t>Création du UserCase et création du diagramme d'activité et de séquence</t>
+  </si>
+  <si>
+    <t>Création du UserCase et mise en place d'un diagramme d'activité, un diagramme de séquence. J'ai commencé à identifier les éléments importans pour constituer un diagramme de séquence.</t>
   </si>
 </sst>
 </file>
@@ -444,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -538,6 +544,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3736,8 +3745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB7A04D-A66F-4A89-83F1-9B353075A776}">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4176,11 +4185,19 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
+    <row r="17" spans="1:18" ht="135" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="7">
+        <v>3</v>
+      </c>
+      <c r="C17" s="35">
+        <v>43915</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -4482,7 +4499,7 @@
       </c>
       <c r="B32" s="14">
         <f>SUM(B16:B31)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>

</xml_diff>

<commit_message>
Journal de travail HM
</commit_message>
<xml_diff>
--- a/LM_Journal_Travail_V1.0.xlsx
+++ b/LM_Journal_Travail_V1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Love-Mirroring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmes\VS2019\Projets\Projet Gerber\Love-Mirroring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9531EC86-20EE-41EE-81D7-02BF88F42C74}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D461B89-FCA9-401B-9218-5E75A20D492E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="NBLecons">#REF!</definedName>
     <definedName name="TachesPlanifiees">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="43">
   <si>
     <t>Jalon</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>Création du UserCase et mise en place d'un diagramme d'activité, un diagramme de séquence. J'ai commencé à identifier les éléments importans pour constituer un diagramme de séquence.</t>
+  </si>
+  <si>
+    <t>MCD</t>
+  </si>
+  <si>
+    <t>25.03.2020</t>
+  </si>
+  <si>
+    <t>Création des premières tables et relations</t>
   </si>
 </sst>
 </file>
@@ -3745,8 +3754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB7A04D-A66F-4A89-83F1-9B353075A776}">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -7935,8 +7944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F222774-5003-490D-9078-78D1F6F89A4A}">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -8397,11 +8406,19 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="9"/>
+    <row r="18" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+      <c r="A18" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="7">
+        <v>2</v>
+      </c>
+      <c r="C18" s="18">
+        <v>43914</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="E18" s="10"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -8418,10 +8435,18 @@
       <c r="R18" s="4"/>
     </row>
     <row r="19" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="A19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="7">
+        <v>4</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="E19" s="10"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -8723,7 +8748,7 @@
       </c>
       <c r="B34" s="14">
         <f>SUM(B18:B33)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
@@ -10044,7 +10069,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B75:B82 B18:B33 B38:B39 B41:B45 B50:B60 B65:B70 B3:B8 B10:B13" xr:uid="{64471589-AB55-4AF0-A3CB-2C4DA302E1FD}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B75:B82 B10:B13 B38:B39 B41:B45 B50:B60 B65:B70 B3:B8 B18:B33" xr:uid="{64471589-AB55-4AF0-A3CB-2C4DA302E1FD}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B83 B34 B46 B61 B71 B14" xr:uid="{E5C4B3DD-C4A0-4BDF-8596-69EE95FDEE2C}">

</xml_diff>

<commit_message>
Modification des UseCases et diagrammes
</commit_message>
<xml_diff>
--- a/LM_Journal_Travail_V1.0.xlsx
+++ b/LM_Journal_Travail_V1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Love-Mirroring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119602E1-582C-4FA3-94CE-8C70C322B854}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4D0B3C-DDDE-4443-B587-26029D593310}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="52">
   <si>
     <t>Jalon</t>
   </si>
@@ -199,6 +199,21 @@
   </si>
   <si>
     <t>Création d'un diagramme de composant qui regroupe les fonctionnalités d'identity server 4. J'ai aussi créé deux diagramme de séquence corresponsant à l'authentification et à la création de compte.</t>
+  </si>
+  <si>
+    <t>Modification des diagrammes de séquence</t>
+  </si>
+  <si>
+    <t>Création de plusieurs diagrammes de séquence pour la gestion du compte de l'utilisateur.</t>
+  </si>
+  <si>
+    <t>Création du diagramme d'état du compte utilisateur</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>Création d'un diagramme d'état pour le compte utilisateur. C'est actuellement un des seuls diagrammes que j'ai pu identifier. Je ne sais pas si celui du paiement pourrait encore entrer en compte.</t>
   </si>
 </sst>
 </file>
@@ -471,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -569,6 +584,9 @@
     </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3767,7 +3785,7 @@
   <dimension ref="A1:R94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3887,7 +3905,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="54" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -3943,7 +3961,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="54" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>14</v>
       </c>
@@ -3971,7 +3989,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" ht="108" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="81" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>16</v>
       </c>
@@ -3999,7 +4017,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="81" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>18</v>
       </c>
@@ -4027,7 +4045,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
@@ -4083,7 +4101,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>22</v>
       </c>
@@ -4178,7 +4196,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>36</v>
       </c>
@@ -4206,7 +4224,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" ht="135" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="81" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>38</v>
       </c>
@@ -4234,7 +4252,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>43</v>
       </c>
@@ -4290,11 +4308,19 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
+    <row r="20" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="36">
+        <v>1.5</v>
+      </c>
+      <c r="C20" s="35">
+        <v>43917</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="E20" s="10"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -4310,11 +4336,19 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
+    <row r="21" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="35">
+        <v>43917</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="E21" s="10"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -4530,13 +4564,13 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B32" s="14">
         <f>SUM(B16:B31)</f>
-        <v>8</v>
+        <v>9.5</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
@@ -4785,7 +4819,7 @@
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
     </row>
-    <row r="44" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="14" t="s">
         <v>22</v>
       </c>
@@ -5100,7 +5134,7 @@
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
     </row>
-    <row r="59" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="14" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Journal de travail Seb+Equipe
</commit_message>
<xml_diff>
--- a/LM_Journal_Travail_V1.0.xlsx
+++ b/LM_Journal_Travail_V1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmes\VS2019\Projets\Projet Gerber\Love-Mirroring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Love-Mirroring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A79D32-745D-4469-8361-2F2830311EBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8510447-E6CD-4677-A0ED-38E8DB2ADA94}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="2955" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="NBLecons">#REF!</definedName>
     <definedName name="TachesPlanifiees">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="91">
   <si>
     <t>Jalon</t>
   </si>
@@ -331,6 +331,15 @@
     <t>Recherche sur les différentes personnalités possible pour le matching
 Création d'un fichier de description clair sur excel</t>
   </si>
+  <si>
+    <t>Adaptation de la création du compte</t>
+  </si>
+  <si>
+    <t>Attribution des tâches</t>
+  </si>
+  <si>
+    <t>J'ai adapté les fonctionnalités qui tourne autour de la création d'un compte. Je m'attaque à la fin de la documentation ce week-end</t>
+  </si>
 </sst>
 </file>
 
@@ -602,7 +611,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -703,6 +712,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -924,8 +936,8 @@
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1330,10 +1342,16 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="18"/>
+    <row r="16" spans="1:18" ht="27.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="7">
+        <v>1</v>
+      </c>
+      <c r="C16" s="18">
+        <v>43914</v>
+      </c>
       <c r="D16" s="9"/>
       <c r="E16" s="10"/>
       <c r="F16" s="4"/>
@@ -1656,7 +1674,7 @@
       </c>
       <c r="B32" s="14">
         <f>SUM(B16:B31)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
@@ -3900,8 +3918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB7A04D-A66F-4A89-83F1-9B353075A776}">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4704,11 +4722,19 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
+    <row r="30" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="7">
+        <v>1</v>
+      </c>
+      <c r="C30" s="35">
+        <v>43925</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="E30" s="10"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -4750,7 +4776,7 @@
       </c>
       <c r="B32" s="14">
         <f>SUM(B16:B31)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
@@ -8186,7 +8212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F222774-5003-490D-9078-78D1F6F89A4A}">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Journal de travail SEB
</commit_message>
<xml_diff>
--- a/LM_Journal_Travail_V1.0.xlsx
+++ b/LM_Journal_Travail_V1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Love-Mirroring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8510447-E6CD-4677-A0ED-38E8DB2ADA94}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B51081-8724-4C5C-952B-2C23A8FDADF6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="93">
   <si>
     <t>Jalon</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>J'ai adapté les fonctionnalités qui tourne autour de la création d'un compte. Je m'attaque à la fin de la documentation ce week-end</t>
+  </si>
+  <si>
+    <t>Ajoute de l'action Reset Password + finalisation des concepts de test</t>
+  </si>
+  <si>
+    <t>J'ai ajouté l'action pour réinitialiser son password et j'ai finaliser le document pour les concepts de test. J'ai aussi exporter les diagrammes en PDF.</t>
   </si>
 </sst>
 </file>
@@ -3918,8 +3924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB7A04D-A66F-4A89-83F1-9B353075A776}">
   <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4587,7 +4593,7 @@
         <v>62</v>
       </c>
       <c r="B25" s="36">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="C25" s="35">
         <v>43920</v>
@@ -4699,7 +4705,7 @@
         <v>71</v>
       </c>
       <c r="B29" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="35">
         <v>43923</v>
@@ -4730,7 +4736,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="35">
-        <v>43925</v>
+        <v>43924</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>90</v>
@@ -4750,11 +4756,19 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
+    <row r="31" spans="1:18" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" s="7">
+        <v>3</v>
+      </c>
+      <c r="C31" s="35">
+        <v>43925</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>92</v>
+      </c>
       <c r="E31" s="10"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -4776,7 +4790,7 @@
       </c>
       <c r="B32" s="14">
         <f>SUM(B16:B31)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>

</xml_diff>

<commit_message>
Finalisation de la documentation - Prêt pour le review
</commit_message>
<xml_diff>
--- a/LM_Journal_Travail_V1.0.xlsx
+++ b/LM_Journal_Travail_V1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmes\VS2019\Projets\Projet Gerber\Love-Mirroring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Love-Mirroring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0F9DEB-F815-4134-A03B-4D9B6C6D19C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797956D0-A36A-4909-B9C8-738439C94DC8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="2955" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="NBLecons">#REF!</definedName>
     <definedName name="TachesPlanifiees">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="101">
   <si>
     <t>Jalon</t>
   </si>
@@ -335,9 +335,6 @@
     <t>Adaptation de la création du compte</t>
   </si>
   <si>
-    <t>Attribution des tâches</t>
-  </si>
-  <si>
     <t>J'ai adapté les fonctionnalités qui tourne autour de la création d'un compte. Je m'attaque à la fin de la documentation ce week-end</t>
   </si>
   <si>
@@ -351,6 +348,27 @@
   </si>
   <si>
     <t>Création du contrôleur du choix des profils</t>
+  </si>
+  <si>
+    <t>24.03.2020 - 07.04.2020</t>
+  </si>
+  <si>
+    <t>Daily SCRUM</t>
+  </si>
+  <si>
+    <t>Daily SCRUM effectué avec l'évaluation des points en cours, en suspens et les éléments qui nécessitaient un Team Review</t>
+  </si>
+  <si>
+    <t>Procès verbal de test - correction + finalisation de la documentation</t>
+  </si>
+  <si>
+    <t>J'ai modifié le procès verbal de test et j'ai finalisé la documentation HERMES. L'équipe effectuera un review sur l'ensemble des documents avant le rendu.</t>
+  </si>
+  <si>
+    <t>Review des documents</t>
+  </si>
+  <si>
+    <t>L'équipe effectue un review global de l'ensemble des documents et éléments de rendu.</t>
   </si>
 </sst>
 </file>
@@ -455,7 +473,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -619,11 +637,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -727,6 +754,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -948,8 +984,8 @@
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1354,17 +1390,19 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" ht="27.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="27" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" s="7">
-        <v>1</v>
-      </c>
-      <c r="C16" s="18">
-        <v>43914</v>
-      </c>
-      <c r="D16" s="9"/>
+        <v>95</v>
+      </c>
+      <c r="B16" s="36">
+        <v>2.5</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1380,11 +1418,19 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
+    <row r="17" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="7">
+        <v>2</v>
+      </c>
+      <c r="C17" s="35">
+        <v>43927</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>100</v>
+      </c>
       <c r="E17" s="10"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -1686,7 +1732,7 @@
       </c>
       <c r="B32" s="14">
         <f>SUM(B16:B31)</f>
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
@@ -3928,10 +3974,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB7A04D-A66F-4A89-83F1-9B353075A776}">
-  <dimension ref="A1:R94"/>
+  <dimension ref="A1:R95"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4745,7 +4791,7 @@
         <v>43924</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="4"/>
@@ -4762,9 +4808,9 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" ht="54" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B31" s="7">
         <v>3</v>
@@ -4773,7 +4819,7 @@
         <v>43925</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E31" s="10"/>
       <c r="F31" s="4"/>
@@ -4790,16 +4836,19 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="14">
-        <f>SUM(B16:B31)</f>
-        <v>33</v>
-      </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
+    <row r="32" spans="1:18" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="38">
+        <v>1</v>
+      </c>
+      <c r="C32" s="39">
+        <v>43926</v>
+      </c>
+      <c r="D32" s="40" t="s">
+        <v>98</v>
+      </c>
       <c r="E32" s="10"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -4816,10 +4865,15 @@
       <c r="R32" s="4"/>
     </row>
     <row r="33" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
+      <c r="A33" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="14">
+        <f>SUM(B16:B32)</f>
+        <v>34</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
       <c r="E33" s="10"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -4835,15 +4889,11 @@
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
     </row>
-    <row r="34" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="2">
-        <v>3</v>
-      </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+    <row r="34" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="16"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
       <c r="E34" s="10"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -4859,17 +4909,15 @@
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="6" t="s">
+    <row r="35" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="2">
         <v>3</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
       <c r="E35" s="10"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -4885,11 +4933,17 @@
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="20"/>
+    <row r="36" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E36" s="10"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -4909,7 +4963,7 @@
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="21"/>
-      <c r="D37" s="9"/>
+      <c r="D37" s="20"/>
       <c r="E37" s="10"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -4928,7 +4982,7 @@
     <row r="38" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
-      <c r="C38" s="22"/>
+      <c r="C38" s="21"/>
       <c r="D38" s="9"/>
       <c r="E38" s="10"/>
       <c r="F38" s="4"/>
@@ -4948,7 +5002,7 @@
     <row r="39" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
-      <c r="C39" s="9"/>
+      <c r="C39" s="22"/>
       <c r="D39" s="9"/>
       <c r="E39" s="10"/>
       <c r="F39" s="4"/>
@@ -5025,11 +5079,11 @@
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
+    <row r="43" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
       <c r="E43" s="10"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -5046,15 +5100,10 @@
       <c r="R43" s="4"/>
     </row>
     <row r="44" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B44" s="14">
-        <f>SUM(B36:B43)</f>
-        <v>0</v>
-      </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
       <c r="E44" s="10"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -5071,10 +5120,15 @@
       <c r="R44" s="4"/>
     </row>
     <row r="45" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="16"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
+      <c r="A45" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="14">
+        <f>SUM(B37:B44)</f>
+        <v>0</v>
+      </c>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
       <c r="E45" s="10"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -5090,15 +5144,11 @@
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
     </row>
-    <row r="46" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" s="2">
-        <v>4</v>
-      </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+    <row r="46" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="16"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
       <c r="E46" s="10"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -5114,17 +5164,15 @@
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
     </row>
-    <row r="47" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5" t="s">
-        <v>5</v>
-      </c>
+    <row r="47" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="2">
+        <v>4</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
       <c r="E47" s="10"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -5140,11 +5188,17 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="48" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A48" s="19"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
+    <row r="48" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E48" s="10"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -5161,10 +5215,10 @@
       <c r="R48" s="4"/>
     </row>
     <row r="49" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
+      <c r="A49" s="19"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
       <c r="E49" s="10"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -5261,10 +5315,10 @@
       <c r="R53" s="4"/>
     </row>
     <row r="54" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A54" s="25"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
       <c r="E54" s="10"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -5340,11 +5394,11 @@
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
     </row>
-    <row r="58" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="23"/>
-      <c r="B58" s="23"/>
-      <c r="C58" s="24"/>
-      <c r="D58" s="24"/>
+    <row r="58" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A58" s="25"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
       <c r="E58" s="10"/>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
@@ -5361,15 +5415,10 @@
       <c r="R58" s="4"/>
     </row>
     <row r="59" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B59" s="14">
-        <f>SUM(B48:B58)</f>
-        <v>0</v>
-      </c>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
+      <c r="A59" s="23"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
       <c r="E59" s="10"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
@@ -5386,10 +5435,15 @@
       <c r="R59" s="4"/>
     </row>
     <row r="60" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="16"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
+      <c r="A60" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" s="14">
+        <f>SUM(B49:B59)</f>
+        <v>0</v>
+      </c>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
       <c r="E60" s="10"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -5405,15 +5459,11 @@
       <c r="Q60" s="4"/>
       <c r="R60" s="4"/>
     </row>
-    <row r="61" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B61" s="2">
-        <v>5</v>
-      </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
+    <row r="61" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="16"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
       <c r="E61" s="10"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
@@ -5429,17 +5479,15 @@
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
     </row>
-    <row r="62" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5" t="s">
+    <row r="62" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="2">
         <v>5</v>
       </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
       <c r="E62" s="10"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
@@ -5455,11 +5503,17 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="63" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="19"/>
-      <c r="B63" s="19"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
+    <row r="63" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E63" s="10"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -5476,10 +5530,10 @@
       <c r="R63" s="4"/>
     </row>
     <row r="64" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
+      <c r="A64" s="19"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
       <c r="E64" s="10"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -5555,11 +5609,11 @@
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
     </row>
-    <row r="68" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="23"/>
-      <c r="B68" s="23"/>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
+    <row r="68" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
       <c r="E68" s="10"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
@@ -5576,15 +5630,10 @@
       <c r="R68" s="4"/>
     </row>
     <row r="69" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B69" s="14">
-        <f>SUM(B63:B68)</f>
-        <v>0</v>
-      </c>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
+      <c r="A69" s="23"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
       <c r="E69" s="10"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -5601,10 +5650,15 @@
       <c r="R69" s="4"/>
     </row>
     <row r="70" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="16"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="16"/>
+      <c r="A70" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B70" s="14">
+        <f>SUM(B64:B69)</f>
+        <v>0</v>
+      </c>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
       <c r="E70" s="10"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -5620,15 +5674,11 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="71" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B71" s="2">
-        <v>6</v>
-      </c>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
+    <row r="71" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="16"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="16"/>
       <c r="E71" s="10"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
@@ -5644,17 +5694,15 @@
       <c r="Q71" s="4"/>
       <c r="R71" s="4"/>
     </row>
-    <row r="72" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5" t="s">
-        <v>5</v>
-      </c>
+    <row r="72" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="2">
+        <v>6</v>
+      </c>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
       <c r="E72" s="10"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
@@ -5670,11 +5718,17 @@
       <c r="Q72" s="4"/>
       <c r="R72" s="4"/>
     </row>
-    <row r="73" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A73" s="19"/>
-      <c r="B73" s="19"/>
-      <c r="C73" s="20"/>
-      <c r="D73" s="20"/>
+    <row r="73" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E73" s="10"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
@@ -5691,10 +5745,10 @@
       <c r="R73" s="4"/>
     </row>
     <row r="74" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A74" s="7"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="9"/>
-      <c r="D74" s="9"/>
+      <c r="A74" s="19"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
       <c r="E74" s="10"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
@@ -5810,11 +5864,11 @@
       <c r="Q79" s="4"/>
       <c r="R79" s="4"/>
     </row>
-    <row r="80" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="23"/>
-      <c r="B80" s="23"/>
-      <c r="C80" s="24"/>
-      <c r="D80" s="24"/>
+    <row r="80" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
       <c r="E80" s="10"/>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
@@ -5831,15 +5885,10 @@
       <c r="R80" s="4"/>
     </row>
     <row r="81" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B81" s="14">
-        <f>SUM(B73:B80)</f>
-        <v>0</v>
-      </c>
-      <c r="C81" s="15"/>
-      <c r="D81" s="15"/>
+      <c r="A81" s="23"/>
+      <c r="B81" s="23"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
       <c r="E81" s="10"/>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
@@ -5855,11 +5904,16 @@
       <c r="Q81" s="4"/>
       <c r="R81" s="4"/>
     </row>
-    <row r="82" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A82" s="16"/>
-      <c r="B82" s="16"/>
-      <c r="C82" s="16"/>
-      <c r="D82" s="16"/>
+    <row r="82" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B82" s="14">
+        <f>SUM(B74:B81)</f>
+        <v>0</v>
+      </c>
+      <c r="C82" s="15"/>
+      <c r="D82" s="15"/>
       <c r="E82" s="10"/>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
@@ -5876,10 +5930,10 @@
       <c r="R82" s="4"/>
     </row>
     <row r="83" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A83" s="27"/>
-      <c r="B83" s="27"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
+      <c r="A83" s="16"/>
+      <c r="B83" s="16"/>
+      <c r="C83" s="16"/>
+      <c r="D83" s="16"/>
       <c r="E83" s="10"/>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
@@ -6096,10 +6150,10 @@
       <c r="R93" s="4"/>
     </row>
     <row r="94" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A94" s="28"/>
-      <c r="B94" s="28"/>
-      <c r="C94" s="28"/>
-      <c r="D94" s="28"/>
+      <c r="A94" s="27"/>
+      <c r="B94" s="27"/>
+      <c r="C94" s="27"/>
+      <c r="D94" s="27"/>
       <c r="E94" s="10"/>
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
@@ -6115,13 +6169,19 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
+    <row r="95" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A95" s="28"/>
+      <c r="B95" s="28"/>
+      <c r="C95" s="28"/>
+      <c r="D95" s="28"/>
+    </row>
   </sheetData>
   <dataValidations xWindow="188" yWindow="522" count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B12 B32 B44 B59 B69 B81" xr:uid="{41F29EDA-D509-4469-8DFB-6A4CE4CEAE07}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B12 B33 B45 B60 B70 B82" xr:uid="{41F29EDA-D509-4469-8DFB-6A4CE4CEAE07}">
       <formula1>0</formula1>
       <formula2>DureePeriode-1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B73:B80 B16:B31 B36:B37 B39:B43 B48:B58 B63:B68 B10:B11 B3:B8" xr:uid="{3039B7E3-952E-4B34-B612-E5A0C049619C}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B74:B81 B37:B38 B40:B44 B49:B59 B64:B69 B10:B11 B3:B8 B16:B32" xr:uid="{3039B7E3-952E-4B34-B612-E5A0C049619C}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -6133,7 +6193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716E2DDB-6361-470B-ACF3-8FDF9046203A}">
   <dimension ref="A1:R95"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
@@ -8232,8 +8292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F222774-5003-490D-9078-78D1F6F89A4A}">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -8982,10 +9042,10 @@
         <v>4.5</v>
       </c>
       <c r="C28" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>94</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="4"/>

</xml_diff>

<commit_message>
Mise à jour de l'incrément
Pour se connecter kelin@lol.ch mdp pour tous les user aB123456*
Pour les autres users voir scriptinsertions
</commit_message>
<xml_diff>
--- a/LM_Journal_Travail_V1.0.xlsx
+++ b/LM_Journal_Travail_V1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Love-Mirroring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmes\VS2019\Projets\Projet Gerber\Love-Mirroring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797956D0-A36A-4909-B9C8-738439C94DC8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4A784D-B79A-4EBD-AE53-95C092752BF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5445" yWindow="2955" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="NBLecons">#REF!</definedName>
     <definedName name="TachesPlanifiees">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="103">
   <si>
     <t>Jalon</t>
   </si>
@@ -369,6 +369,13 @@
   </si>
   <si>
     <t>L'équipe effectue un review global de l'ensemble des documents et éléments de rendu.</t>
+  </si>
+  <si>
+    <t>05.04.2020</t>
+  </si>
+  <si>
+    <t>Affichage des filtres
+Affichage des profils correspondant aux filtres</t>
   </si>
 </sst>
 </file>
@@ -984,7 +991,7 @@
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -8292,8 +8299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F222774-5003-490D-9078-78D1F6F89A4A}">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -9062,11 +9069,19 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
+    <row r="29" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="7">
+        <v>8</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="E29" s="10"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -9168,7 +9183,7 @@
       </c>
       <c r="B34" s="14">
         <f>SUM(B18:B33)</f>
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>

</xml_diff>

<commit_message>
Update Journal Travail Seb
</commit_message>
<xml_diff>
--- a/LM_Journal_Travail_V1.0.xlsx
+++ b/LM_Journal_Travail_V1.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositories\Love-Mirroring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Love-Mirroring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8784CF9B-CB10-4657-A56D-3E108FA60BFA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838EAE48-CC6D-429C-A0B6-E95E6885AE57}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="144">
   <si>
     <t>Jalon</t>
   </si>
@@ -494,6 +494,12 @@
   </si>
   <si>
     <t>Elaboration qualité et concept de d'exploitation</t>
+  </si>
+  <si>
+    <t>Correction des user stories + usecase + diagramme</t>
+  </si>
+  <si>
+    <t>Suite à une conversation avec Monsieur Gerber, je me suis rendu compte qu'on faisait fausse route sur les user stories j'ai donc effectué les corrections nécessaire pour avoir un bon rendu.</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1116,7 @@
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4099,10 +4105,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB7A04D-A66F-4A89-83F1-9B353075A776}">
-  <dimension ref="A1:R95"/>
+  <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -4961,7 +4967,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="1:18" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" ht="54" x14ac:dyDescent="0.3">
       <c r="A32" s="38" t="s">
         <v>97</v>
       </c>
@@ -4989,16 +4995,19 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="33" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="14">
-        <f>SUM(B16:B32)</f>
-        <v>34</v>
-      </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
+    <row r="33" spans="1:18" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" s="38">
+        <v>3</v>
+      </c>
+      <c r="C33" s="39">
+        <v>43927</v>
+      </c>
+      <c r="D33" s="40" t="s">
+        <v>143</v>
+      </c>
       <c r="E33" s="10"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -5015,10 +5024,15 @@
       <c r="R33" s="4"/>
     </row>
     <row r="34" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
+      <c r="A34" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="14">
+        <f>SUM(B16:B33)</f>
+        <v>37</v>
+      </c>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
       <c r="E34" s="10"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
@@ -5034,15 +5048,11 @@
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="2">
-        <v>3</v>
-      </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+    <row r="35" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
       <c r="E35" s="10"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -5058,17 +5068,15 @@
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="6" t="s">
+    <row r="36" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="2">
         <v>3</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
       <c r="E36" s="10"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -5084,11 +5092,17 @@
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
     </row>
-    <row r="37" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="20"/>
+    <row r="37" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E37" s="10"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -5108,7 +5122,7 @@
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="21"/>
-      <c r="D38" s="9"/>
+      <c r="D38" s="20"/>
       <c r="E38" s="10"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -5127,7 +5141,7 @@
     <row r="39" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
-      <c r="C39" s="22"/>
+      <c r="C39" s="21"/>
       <c r="D39" s="9"/>
       <c r="E39" s="10"/>
       <c r="F39" s="4"/>
@@ -5147,7 +5161,7 @@
     <row r="40" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
-      <c r="C40" s="9"/>
+      <c r="C40" s="22"/>
       <c r="D40" s="9"/>
       <c r="E40" s="10"/>
       <c r="F40" s="4"/>
@@ -5224,11 +5238,11 @@
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
     </row>
-    <row r="44" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
+    <row r="44" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
       <c r="E44" s="10"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -5245,15 +5259,10 @@
       <c r="R44" s="4"/>
     </row>
     <row r="45" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45" s="14">
-        <f>SUM(B37:B44)</f>
-        <v>0</v>
-      </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
       <c r="E45" s="10"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -5270,10 +5279,15 @@
       <c r="R45" s="4"/>
     </row>
     <row r="46" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="16"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
+      <c r="A46" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="14">
+        <f>SUM(B38:B45)</f>
+        <v>0</v>
+      </c>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
       <c r="E46" s="10"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -5289,15 +5303,11 @@
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
     </row>
-    <row r="47" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="2">
-        <v>4</v>
-      </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+    <row r="47" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
       <c r="E47" s="10"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -5313,17 +5323,15 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="48" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5" t="s">
-        <v>5</v>
-      </c>
+    <row r="48" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="2">
+        <v>4</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
       <c r="E48" s="10"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -5339,11 +5347,17 @@
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
     </row>
-    <row r="49" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A49" s="19"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
+    <row r="49" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E49" s="10"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -5360,10 +5374,10 @@
       <c r="R49" s="4"/>
     </row>
     <row r="50" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
+      <c r="A50" s="19"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
       <c r="E50" s="10"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
@@ -5460,10 +5474,10 @@
       <c r="R54" s="4"/>
     </row>
     <row r="55" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A55" s="25"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
       <c r="E55" s="10"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -5539,11 +5553,11 @@
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
     </row>
-    <row r="59" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="23"/>
-      <c r="B59" s="23"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="24"/>
+    <row r="59" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A59" s="25"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
       <c r="E59" s="10"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
@@ -5560,15 +5574,10 @@
       <c r="R59" s="4"/>
     </row>
     <row r="60" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B60" s="14">
-        <f>SUM(B49:B59)</f>
-        <v>0</v>
-      </c>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
+      <c r="A60" s="23"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="24"/>
       <c r="E60" s="10"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -5585,10 +5594,15 @@
       <c r="R60" s="4"/>
     </row>
     <row r="61" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="16"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
+      <c r="A61" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" s="14">
+        <f>SUM(B50:B60)</f>
+        <v>0</v>
+      </c>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
       <c r="E61" s="10"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
@@ -5604,15 +5618,11 @@
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
     </row>
-    <row r="62" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B62" s="2">
-        <v>5</v>
-      </c>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+    <row r="62" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="16"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
       <c r="E62" s="10"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
@@ -5628,17 +5638,15 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="63" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5" t="s">
+    <row r="63" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B63" s="2">
         <v>5</v>
       </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
       <c r="E63" s="10"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -5654,11 +5662,17 @@
       <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
     </row>
-    <row r="64" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A64" s="19"/>
-      <c r="B64" s="19"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
+    <row r="64" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E64" s="10"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -5675,10 +5689,10 @@
       <c r="R64" s="4"/>
     </row>
     <row r="65" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="9"/>
+      <c r="A65" s="19"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20"/>
       <c r="E65" s="10"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
@@ -5754,11 +5768,11 @@
       <c r="Q68" s="4"/>
       <c r="R68" s="4"/>
     </row>
-    <row r="69" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="23"/>
-      <c r="B69" s="23"/>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
+    <row r="69" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
       <c r="E69" s="10"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -5775,15 +5789,10 @@
       <c r="R69" s="4"/>
     </row>
     <row r="70" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B70" s="14">
-        <f>SUM(B64:B69)</f>
-        <v>0</v>
-      </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
+      <c r="A70" s="23"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="24"/>
       <c r="E70" s="10"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -5800,10 +5809,15 @@
       <c r="R70" s="4"/>
     </row>
     <row r="71" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="16"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="16"/>
-      <c r="D71" s="16"/>
+      <c r="A71" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B71" s="14">
+        <f>SUM(B65:B70)</f>
+        <v>0</v>
+      </c>
+      <c r="C71" s="15"/>
+      <c r="D71" s="15"/>
       <c r="E71" s="10"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
@@ -5819,15 +5833,11 @@
       <c r="Q71" s="4"/>
       <c r="R71" s="4"/>
     </row>
-    <row r="72" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B72" s="2">
-        <v>6</v>
-      </c>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
+    <row r="72" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="16"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="16"/>
       <c r="E72" s="10"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
@@ -5843,17 +5853,15 @@
       <c r="Q72" s="4"/>
       <c r="R72" s="4"/>
     </row>
-    <row r="73" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5" t="s">
-        <v>5</v>
-      </c>
+    <row r="73" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73" s="2">
+        <v>6</v>
+      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
       <c r="E73" s="10"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
@@ -5869,11 +5877,17 @@
       <c r="Q73" s="4"/>
       <c r="R73" s="4"/>
     </row>
-    <row r="74" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A74" s="19"/>
-      <c r="B74" s="19"/>
-      <c r="C74" s="20"/>
-      <c r="D74" s="20"/>
+    <row r="74" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E74" s="10"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
@@ -5890,10 +5904,10 @@
       <c r="R74" s="4"/>
     </row>
     <row r="75" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A75" s="7"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="9"/>
-      <c r="D75" s="9"/>
+      <c r="A75" s="19"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="20"/>
       <c r="E75" s="10"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
@@ -6009,11 +6023,11 @@
       <c r="Q80" s="4"/>
       <c r="R80" s="4"/>
     </row>
-    <row r="81" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="23"/>
-      <c r="B81" s="23"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
+    <row r="81" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
       <c r="E81" s="10"/>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
@@ -6030,15 +6044,10 @@
       <c r="R81" s="4"/>
     </row>
     <row r="82" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B82" s="14">
-        <f>SUM(B74:B81)</f>
-        <v>0</v>
-      </c>
-      <c r="C82" s="15"/>
-      <c r="D82" s="15"/>
+      <c r="A82" s="23"/>
+      <c r="B82" s="23"/>
+      <c r="C82" s="24"/>
+      <c r="D82" s="24"/>
       <c r="E82" s="10"/>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
@@ -6054,11 +6063,16 @@
       <c r="Q82" s="4"/>
       <c r="R82" s="4"/>
     </row>
-    <row r="83" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A83" s="16"/>
-      <c r="B83" s="16"/>
-      <c r="C83" s="16"/>
-      <c r="D83" s="16"/>
+    <row r="83" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B83" s="14">
+        <f>SUM(B75:B82)</f>
+        <v>0</v>
+      </c>
+      <c r="C83" s="15"/>
+      <c r="D83" s="15"/>
       <c r="E83" s="10"/>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
@@ -6075,10 +6089,10 @@
       <c r="R83" s="4"/>
     </row>
     <row r="84" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A84" s="27"/>
-      <c r="B84" s="27"/>
-      <c r="C84" s="27"/>
-      <c r="D84" s="27"/>
+      <c r="A84" s="16"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="16"/>
       <c r="E84" s="10"/>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
@@ -6295,18 +6309,38 @@
       <c r="R94" s="4"/>
     </row>
     <row r="95" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A95" s="28"/>
-      <c r="B95" s="28"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="28"/>
+      <c r="A95" s="27"/>
+      <c r="B95" s="27"/>
+      <c r="C95" s="27"/>
+      <c r="D95" s="27"/>
+      <c r="E95" s="10"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="4"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="4"/>
+      <c r="L95" s="4"/>
+      <c r="M95" s="4"/>
+      <c r="N95" s="4"/>
+      <c r="O95" s="4"/>
+      <c r="P95" s="4"/>
+      <c r="Q95" s="4"/>
+      <c r="R95" s="4"/>
+    </row>
+    <row r="96" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A96" s="28"/>
+      <c r="B96" s="28"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="28"/>
     </row>
   </sheetData>
   <dataValidations xWindow="188" yWindow="522" count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B12 B33 B45 B60 B70 B82" xr:uid="{41F29EDA-D509-4469-8DFB-6A4CE4CEAE07}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B12 B34 B46 B61 B71 B83" xr:uid="{41F29EDA-D509-4469-8DFB-6A4CE4CEAE07}">
       <formula1>0</formula1>
       <formula2>DureePeriode-1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B74:B81 B37:B38 B40:B44 B49:B59 B64:B69 B10:B11 B3:B8 B16:B32" xr:uid="{3039B7E3-952E-4B34-B612-E5A0C049619C}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B75:B82 B38:B39 B41:B45 B50:B60 B65:B70 B10:B11 B3:B8 B16:B33" xr:uid="{3039B7E3-952E-4B34-B612-E5A0C049619C}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -6318,7 +6352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716E2DDB-6361-470B-ACF3-8FDF9046203A}">
   <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
@@ -8003,7 +8037,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="71" spans="1:18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="9"/>

</xml_diff>

<commit_message>
Journal HM + changement relation userroles
</commit_message>
<xml_diff>
--- a/LM_Journal_Travail_V1.0.xlsx
+++ b/LM_Journal_Travail_V1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmes\VS2019\Projets\Projet Gerber\Love-Mirroring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1338F63-D9E1-4BC9-AC51-E51FFC33751F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2839157A-147B-48EA-870B-84E468005374}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="2115" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="189">
   <si>
     <t>Jalon</t>
   </si>
@@ -635,14 +635,22 @@
     <t>Création d'un controlleur pour chercher des titres en fonction de leur titre. Je dois trouver un autre moyen de chercher des musiques et je dois réfléchir à la manière de l'implémenter dans l'application. Je peux récupérer facilement des pistes si je mets des mots-clés. J'ai aussi changer un peu la structure du projet MVC pour regrouper les liens sur la gestion du compte de l'utilisateur. Je vais continuer mon développement sur Spotify et entrer en phase de test pour mon développement.</t>
   </si>
   <si>
-    <t>06.05.202</t>
-  </si>
-  <si>
     <t>Amélioration des tâches précèdentes (Gestion des exceptions)
 Gestion des rôles commencé
 Afficher rôles Ok
 Créer rôle Ok
 Ajouter rôle a un utilisateur en attente</t>
+  </si>
+  <si>
+    <t>07.05.2020</t>
+  </si>
+  <si>
+    <t>06.05.2020</t>
+  </si>
+  <si>
+    <t>Ajout d'un rôle à un utilisateur OK
+Supprimer un rôle d'un utilisateur OK
+Ajout des Autororize sur les controlluers en attente</t>
   </si>
 </sst>
 </file>
@@ -9067,8 +9075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F222774-5003-490D-9078-78D1F6F89A4A}">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -10224,10 +10232,10 @@
         <v>9</v>
       </c>
       <c r="C44" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D44" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>186</v>
       </c>
       <c r="E44" s="10"/>
       <c r="F44" s="4"/>
@@ -10244,11 +10252,19 @@
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
     </row>
-    <row r="45" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
+    <row r="45" spans="1:18" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" s="23">
+        <v>9</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>188</v>
+      </c>
       <c r="E45" s="10"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -10270,7 +10286,7 @@
       </c>
       <c r="B46" s="14">
         <f>SUM(B38:B45)</f>
-        <v>33.5</v>
+        <v>42.5</v>
       </c>
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>

</xml_diff>

<commit_message>
Journal de travail Paul
</commit_message>
<xml_diff>
--- a/LM_Journal_Travail_V1.0.xlsx
+++ b/LM_Journal_Travail_V1.0.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Love-Mirroring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Documents\GitHub\Love-Mirroring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188607D5-9CD6-4FBE-9D13-8FED3E4A444B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA5C19A-794A-4D38-BDFD-879283793BA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="1" r:id="rId1"/>
     <sheet name="Sébastien Berger" sheetId="4" r:id="rId2"/>
     <sheet name="Tim Allemann" sheetId="8" r:id="rId3"/>
     <sheet name="Hans Morsch" sheetId="9" r:id="rId4"/>
+    <sheet name="Paul Gillet" sheetId="10" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_Toc493855087" localSheetId="3">'Hans Morsch'!$A$12</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="257">
   <si>
     <t>Jalon</t>
   </si>
@@ -834,6 +835,33 @@
   </si>
   <si>
     <t>J'ai implémenté une extension javascript pour le datepicker avec l'aide de Monsieur Allemann car il avait déjà utilisé ça dans un ancien projet. J'ai eu quelques soucis au niveau du format mais maintenant le plugin marche.</t>
+  </si>
+  <si>
+    <t>Reprise du projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Présentation des choses qui ont été faites et assignation à des tâches.
+Explication de ce qui doit être fait.
+</t>
+  </si>
+  <si>
+    <t>Création avec l'api du CRUD pour les sexes côté admin.
+Affichage des Sexes, affichage des détails</t>
+  </si>
+  <si>
+    <t>Modification et suppression des Sexes</t>
+  </si>
+  <si>
+    <t>Modification interface administration - Finalisation CRUD Sexes</t>
+  </si>
+  <si>
+    <t>Modification interface administration -Commencement CRUD Sexes</t>
+  </si>
+  <si>
+    <t>Modification interface administration - CRUD Sexualités</t>
+  </si>
+  <si>
+    <t>25,05,20</t>
   </si>
 </sst>
 </file>
@@ -1546,20 +1574,20 @@
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="78.42578125" customWidth="1"/>
-    <col min="5" max="6" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="78.44140625" customWidth="1"/>
+    <col min="5" max="6" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1585,7 +1613,7 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -1613,7 +1641,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -1641,7 +1669,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -1669,7 +1697,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1697,7 +1725,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
@@ -1725,7 +1753,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>14</v>
       </c>
@@ -1753,7 +1781,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>16</v>
       </c>
@@ -1781,7 +1809,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>18</v>
       </c>
@@ -1809,7 +1837,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
@@ -1837,7 +1865,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
@@ -1857,7 +1885,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>22</v>
       </c>
@@ -1882,7 +1910,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -1902,7 +1930,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1926,7 +1954,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>2</v>
       </c>
@@ -1952,7 +1980,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
         <v>95</v>
       </c>
@@ -1980,7 +2008,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>99</v>
       </c>
@@ -2008,7 +2036,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="9"/>
@@ -2028,7 +2056,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="9"/>
@@ -2048,7 +2076,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="9"/>
@@ -4538,18 +4566,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB7A04D-A66F-4A89-83F1-9B353075A776}">
   <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4575,7 +4603,7 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -4603,7 +4631,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -4631,7 +4659,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -4659,7 +4687,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -4687,7 +4715,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
@@ -4715,7 +4743,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>14</v>
       </c>
@@ -4743,7 +4771,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>16</v>
       </c>
@@ -4771,7 +4799,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>18</v>
       </c>
@@ -4799,7 +4827,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
@@ -4827,7 +4855,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
@@ -4855,7 +4883,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>22</v>
       </c>
@@ -4880,7 +4908,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -4900,7 +4928,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -4924,7 +4952,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>2</v>
       </c>
@@ -4950,7 +4978,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>36</v>
       </c>
@@ -4978,7 +5006,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>38</v>
       </c>
@@ -5006,7 +5034,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>42</v>
       </c>
@@ -5034,7 +5062,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
@@ -5062,7 +5090,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>46</v>
       </c>
@@ -5090,7 +5118,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>48</v>
       </c>
@@ -5118,7 +5146,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>50</v>
       </c>
@@ -5146,7 +5174,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18" ht="121.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>73</v>
       </c>
@@ -5174,7 +5202,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>52</v>
       </c>
@@ -5202,7 +5230,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>62</v>
       </c>
@@ -5230,7 +5258,7 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
     </row>
-    <row r="26" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>63</v>
       </c>
@@ -5258,7 +5286,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>65</v>
       </c>
@@ -5286,7 +5314,7 @@
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>69</v>
       </c>
@@ -5314,7 +5342,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>71</v>
       </c>
@@ -5342,7 +5370,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>88</v>
       </c>
@@ -5370,7 +5398,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>90</v>
       </c>
@@ -5398,7 +5426,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A32" s="38" t="s">
         <v>97</v>
       </c>
@@ -5426,7 +5454,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="33" spans="1:18" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="38" t="s">
         <v>142</v>
       </c>
@@ -5454,7 +5482,7 @@
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
     </row>
-    <row r="34" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
         <v>22</v>
       </c>
@@ -5479,7 +5507,7 @@
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -5499,7 +5527,7 @@
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -5523,7 +5551,7 @@
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
     </row>
-    <row r="37" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>2</v>
       </c>
@@ -5549,7 +5577,7 @@
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
     </row>
-    <row r="38" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>148</v>
       </c>
@@ -5577,7 +5605,7 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>150</v>
       </c>
@@ -5605,7 +5633,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="40" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>152</v>
       </c>
@@ -5633,7 +5661,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>154</v>
       </c>
@@ -5661,7 +5689,7 @@
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
     </row>
-    <row r="42" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>156</v>
       </c>
@@ -5689,7 +5717,7 @@
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>158</v>
       </c>
@@ -5717,7 +5745,7 @@
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
     </row>
-    <row r="44" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>165</v>
       </c>
@@ -5745,7 +5773,7 @@
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
     </row>
-    <row r="45" spans="1:18" ht="81.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="23" t="s">
         <v>167</v>
       </c>
@@ -5773,7 +5801,7 @@
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
     </row>
-    <row r="46" spans="1:18" ht="108.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" ht="106.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="23" t="s">
         <v>169</v>
       </c>
@@ -5801,7 +5829,7 @@
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
     </row>
-    <row r="47" spans="1:18" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="42" t="s">
         <v>171</v>
       </c>
@@ -5829,7 +5857,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="48" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="42" t="s">
         <v>173</v>
       </c>
@@ -5857,7 +5885,7 @@
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
     </row>
-    <row r="49" spans="1:18" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="42" t="s">
         <v>181</v>
       </c>
@@ -5885,7 +5913,7 @@
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
     </row>
-    <row r="50" spans="1:18" ht="81.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:18" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="42" t="s">
         <v>183</v>
       </c>
@@ -5913,7 +5941,7 @@
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
     </row>
-    <row r="51" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="42" t="s">
         <v>189</v>
       </c>
@@ -5941,7 +5969,7 @@
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
     </row>
-    <row r="52" spans="1:18" ht="68.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:18" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="42" t="s">
         <v>191</v>
       </c>
@@ -5969,7 +5997,7 @@
       <c r="Q52" s="4"/>
       <c r="R52" s="4"/>
     </row>
-    <row r="53" spans="1:18" ht="81.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="42" t="s">
         <v>195</v>
       </c>
@@ -5997,7 +6025,7 @@
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
     </row>
-    <row r="54" spans="1:18" ht="81.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="42" t="s">
         <v>197</v>
       </c>
@@ -6025,7 +6053,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="55" spans="1:18" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:18" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="42" t="s">
         <v>243</v>
       </c>
@@ -6053,7 +6081,7 @@
       <c r="Q55" s="4"/>
       <c r="R55" s="4"/>
     </row>
-    <row r="56" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="14" t="s">
         <v>22</v>
       </c>
@@ -6078,7 +6106,7 @@
       <c r="Q56" s="4"/>
       <c r="R56" s="4"/>
     </row>
-    <row r="57" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="16"/>
       <c r="B57" s="16"/>
       <c r="C57" s="16"/>
@@ -6098,7 +6126,7 @@
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
     </row>
-    <row r="58" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
@@ -6122,7 +6150,7 @@
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
     </row>
-    <row r="59" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>2</v>
       </c>
@@ -6148,7 +6176,7 @@
       <c r="Q59" s="4"/>
       <c r="R59" s="4"/>
     </row>
-    <row r="60" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A60" s="19" t="s">
         <v>245</v>
       </c>
@@ -6176,7 +6204,7 @@
       <c r="Q60" s="4"/>
       <c r="R60" s="4"/>
     </row>
-    <row r="61" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A61" s="58" t="s">
         <v>245</v>
       </c>
@@ -6204,7 +6232,7 @@
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
     </row>
-    <row r="62" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>245</v>
       </c>
@@ -6232,7 +6260,7 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="63" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="9"/>
@@ -6252,7 +6280,7 @@
       <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
     </row>
-    <row r="64" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="9"/>
@@ -6272,7 +6300,7 @@
       <c r="Q64" s="4"/>
       <c r="R64" s="4"/>
     </row>
-    <row r="65" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="9"/>
@@ -6292,7 +6320,7 @@
       <c r="Q65" s="4"/>
       <c r="R65" s="4"/>
     </row>
-    <row r="66" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="9"/>
@@ -6312,7 +6340,7 @@
       <c r="Q66" s="4"/>
       <c r="R66" s="4"/>
     </row>
-    <row r="67" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A67" s="25"/>
       <c r="B67" s="25"/>
       <c r="C67" s="26"/>
@@ -6332,7 +6360,7 @@
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
     </row>
-    <row r="68" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A68" s="25"/>
       <c r="B68" s="25"/>
       <c r="C68" s="26"/>
@@ -6352,7 +6380,7 @@
       <c r="Q68" s="4"/>
       <c r="R68" s="4"/>
     </row>
-    <row r="69" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A69" s="25"/>
       <c r="B69" s="25"/>
       <c r="C69" s="26"/>
@@ -6372,7 +6400,7 @@
       <c r="Q69" s="4"/>
       <c r="R69" s="4"/>
     </row>
-    <row r="70" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A70" s="25"/>
       <c r="B70" s="25"/>
       <c r="C70" s="26"/>
@@ -6392,7 +6420,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="71" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="23"/>
       <c r="B71" s="23"/>
       <c r="C71" s="24"/>
@@ -6412,7 +6440,7 @@
       <c r="Q71" s="4"/>
       <c r="R71" s="4"/>
     </row>
-    <row r="72" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="14" t="s">
         <v>22</v>
       </c>
@@ -6437,7 +6465,7 @@
       <c r="Q72" s="4"/>
       <c r="R72" s="4"/>
     </row>
-    <row r="73" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="16"/>
       <c r="B73" s="16"/>
       <c r="C73" s="16"/>
@@ -6457,7 +6485,7 @@
       <c r="Q73" s="4"/>
       <c r="R73" s="4"/>
     </row>
-    <row r="74" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>0</v>
       </c>
@@ -6481,7 +6509,7 @@
       <c r="Q74" s="4"/>
       <c r="R74" s="4"/>
     </row>
-    <row r="75" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>2</v>
       </c>
@@ -6507,7 +6535,7 @@
       <c r="Q75" s="4"/>
       <c r="R75" s="4"/>
     </row>
-    <row r="76" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A76" s="19"/>
       <c r="B76" s="19"/>
       <c r="C76" s="20"/>
@@ -6527,7 +6555,7 @@
       <c r="Q76" s="4"/>
       <c r="R76" s="4"/>
     </row>
-    <row r="77" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="9"/>
@@ -6547,7 +6575,7 @@
       <c r="Q77" s="4"/>
       <c r="R77" s="4"/>
     </row>
-    <row r="78" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="9"/>
@@ -6567,7 +6595,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="79" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="9"/>
@@ -6587,7 +6615,7 @@
       <c r="Q79" s="4"/>
       <c r="R79" s="4"/>
     </row>
-    <row r="80" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="9"/>
@@ -6607,7 +6635,7 @@
       <c r="Q80" s="4"/>
       <c r="R80" s="4"/>
     </row>
-    <row r="81" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="23"/>
       <c r="B81" s="23"/>
       <c r="C81" s="24"/>
@@ -6627,7 +6655,7 @@
       <c r="Q81" s="4"/>
       <c r="R81" s="4"/>
     </row>
-    <row r="82" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="14" t="s">
         <v>22</v>
       </c>
@@ -6652,7 +6680,7 @@
       <c r="Q82" s="4"/>
       <c r="R82" s="4"/>
     </row>
-    <row r="83" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="16"/>
       <c r="B83" s="16"/>
       <c r="C83" s="16"/>
@@ -6672,7 +6700,7 @@
       <c r="Q83" s="4"/>
       <c r="R83" s="4"/>
     </row>
-    <row r="84" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
@@ -6696,7 +6724,7 @@
       <c r="Q84" s="4"/>
       <c r="R84" s="4"/>
     </row>
-    <row r="85" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>2</v>
       </c>
@@ -6722,7 +6750,7 @@
       <c r="Q85" s="4"/>
       <c r="R85" s="4"/>
     </row>
-    <row r="86" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A86" s="19"/>
       <c r="B86" s="19"/>
       <c r="C86" s="20"/>
@@ -6742,7 +6770,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="87" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="9"/>
@@ -6762,7 +6790,7 @@
       <c r="Q87" s="4"/>
       <c r="R87" s="4"/>
     </row>
-    <row r="88" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="9"/>
@@ -6782,7 +6810,7 @@
       <c r="Q88" s="4"/>
       <c r="R88" s="4"/>
     </row>
-    <row r="89" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="9"/>
@@ -6802,7 +6830,7 @@
       <c r="Q89" s="4"/>
       <c r="R89" s="4"/>
     </row>
-    <row r="90" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="9"/>
@@ -6822,7 +6850,7 @@
       <c r="Q90" s="4"/>
       <c r="R90" s="4"/>
     </row>
-    <row r="91" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="9"/>
@@ -6842,7 +6870,7 @@
       <c r="Q91" s="4"/>
       <c r="R91" s="4"/>
     </row>
-    <row r="92" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="9"/>
@@ -6862,7 +6890,7 @@
       <c r="Q92" s="4"/>
       <c r="R92" s="4"/>
     </row>
-    <row r="93" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="23"/>
       <c r="B93" s="23"/>
       <c r="C93" s="24"/>
@@ -6882,7 +6910,7 @@
       <c r="Q93" s="4"/>
       <c r="R93" s="4"/>
     </row>
-    <row r="94" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="14" t="s">
         <v>22</v>
       </c>
@@ -6907,7 +6935,7 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="95" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A95" s="16"/>
       <c r="B95" s="16"/>
       <c r="C95" s="16"/>
@@ -6927,7 +6955,7 @@
       <c r="Q95" s="4"/>
       <c r="R95" s="4"/>
     </row>
-    <row r="96" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A96" s="27"/>
       <c r="B96" s="27"/>
       <c r="C96" s="27"/>
@@ -6947,7 +6975,7 @@
       <c r="Q96" s="4"/>
       <c r="R96" s="4"/>
     </row>
-    <row r="97" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A97" s="27"/>
       <c r="B97" s="27"/>
       <c r="C97" s="27"/>
@@ -6967,7 +6995,7 @@
       <c r="Q97" s="4"/>
       <c r="R97" s="4"/>
     </row>
-    <row r="98" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A98" s="27"/>
       <c r="B98" s="27"/>
       <c r="C98" s="27"/>
@@ -6987,7 +7015,7 @@
       <c r="Q98" s="4"/>
       <c r="R98" s="4"/>
     </row>
-    <row r="99" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A99" s="27"/>
       <c r="B99" s="27"/>
       <c r="C99" s="27"/>
@@ -7007,7 +7035,7 @@
       <c r="Q99" s="4"/>
       <c r="R99" s="4"/>
     </row>
-    <row r="100" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A100" s="27"/>
       <c r="B100" s="27"/>
       <c r="C100" s="27"/>
@@ -7027,7 +7055,7 @@
       <c r="Q100" s="4"/>
       <c r="R100" s="4"/>
     </row>
-    <row r="101" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A101" s="27"/>
       <c r="B101" s="27"/>
       <c r="C101" s="27"/>
@@ -7047,7 +7075,7 @@
       <c r="Q101" s="4"/>
       <c r="R101" s="4"/>
     </row>
-    <row r="102" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A102" s="27"/>
       <c r="B102" s="27"/>
       <c r="C102" s="27"/>
@@ -7067,7 +7095,7 @@
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
     </row>
-    <row r="103" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A103" s="27"/>
       <c r="B103" s="27"/>
       <c r="C103" s="27"/>
@@ -7087,7 +7115,7 @@
       <c r="Q103" s="4"/>
       <c r="R103" s="4"/>
     </row>
-    <row r="104" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A104" s="27"/>
       <c r="B104" s="27"/>
       <c r="C104" s="27"/>
@@ -7107,7 +7135,7 @@
       <c r="Q104" s="4"/>
       <c r="R104" s="4"/>
     </row>
-    <row r="105" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A105" s="27"/>
       <c r="B105" s="27"/>
       <c r="C105" s="27"/>
@@ -7127,13 +7155,13 @@
       <c r="Q105" s="4"/>
       <c r="R105" s="4"/>
     </row>
-    <row r="106" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A106" s="27"/>
       <c r="B106" s="27"/>
       <c r="C106" s="27"/>
       <c r="D106" s="27"/>
     </row>
-    <row r="107" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A107" s="28"/>
       <c r="B107" s="28"/>
       <c r="C107" s="28"/>
@@ -7157,18 +7185,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716E2DDB-6361-470B-ACF3-8FDF9046203A}">
   <dimension ref="A1:R117"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7194,7 +7222,7 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -7222,7 +7250,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -7250,7 +7278,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -7278,7 +7306,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -7306,7 +7334,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
@@ -7334,7 +7362,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>14</v>
       </c>
@@ -7362,7 +7390,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" ht="108" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>16</v>
       </c>
@@ -7390,7 +7418,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>18</v>
       </c>
@@ -7418,7 +7446,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
@@ -7446,7 +7474,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -7472,7 +7500,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -7498,7 +7526,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>22</v>
       </c>
@@ -7523,7 +7551,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -7543,7 +7571,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -7593,7 +7621,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>103</v>
       </c>
@@ -7619,7 +7647,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>105</v>
       </c>
@@ -7643,7 +7671,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>106</v>
       </c>
@@ -7669,7 +7697,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>108</v>
       </c>
@@ -7695,7 +7723,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>110</v>
       </c>
@@ -7721,7 +7749,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>112</v>
       </c>
@@ -7747,7 +7775,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>114</v>
       </c>
@@ -7773,7 +7801,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="1:18" ht="108" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>116</v>
       </c>
@@ -7799,7 +7827,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>118</v>
       </c>
@@ -7825,7 +7853,7 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
     </row>
-    <row r="26" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>120</v>
       </c>
@@ -7851,7 +7879,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" ht="121.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>122</v>
       </c>
@@ -7877,7 +7905,7 @@
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>124</v>
       </c>
@@ -7903,7 +7931,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>126</v>
       </c>
@@ -7929,7 +7957,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>124</v>
       </c>
@@ -7955,7 +7983,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>129</v>
       </c>
@@ -7981,7 +8009,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>131</v>
       </c>
@@ -8007,7 +8035,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="33" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>133</v>
       </c>
@@ -8033,7 +8061,7 @@
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
     </row>
-    <row r="34" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>134</v>
       </c>
@@ -8059,7 +8087,7 @@
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>136</v>
       </c>
@@ -8085,7 +8113,7 @@
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>138</v>
       </c>
@@ -8111,7 +8139,7 @@
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
     </row>
-    <row r="37" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>140</v>
       </c>
@@ -8137,7 +8165,7 @@
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
     </row>
-    <row r="38" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="9"/>
@@ -8157,7 +8185,7 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="14" t="s">
         <v>22</v>
       </c>
@@ -8182,7 +8210,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="40" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -8202,7 +8230,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -8226,7 +8254,7 @@
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
     </row>
-    <row r="42" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>2</v>
       </c>
@@ -8252,7 +8280,7 @@
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="1:18" s="50" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" s="50" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A43" s="33" t="s">
         <v>202</v>
       </c>
@@ -8276,7 +8304,7 @@
       <c r="Q43" s="49"/>
       <c r="R43" s="49"/>
     </row>
-    <row r="44" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A44" s="33" t="s">
         <v>203</v>
       </c>
@@ -8302,7 +8330,7 @@
       <c r="Q44" s="49"/>
       <c r="R44" s="49"/>
     </row>
-    <row r="45" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A45" s="33" t="s">
         <v>205</v>
       </c>
@@ -8326,7 +8354,7 @@
       <c r="Q45" s="49"/>
       <c r="R45" s="49"/>
     </row>
-    <row r="46" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A46" s="33" t="s">
         <v>206</v>
       </c>
@@ -8350,7 +8378,7 @@
       <c r="Q46" s="49"/>
       <c r="R46" s="49"/>
     </row>
-    <row r="47" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A47" s="33" t="s">
         <v>207</v>
       </c>
@@ -8374,7 +8402,7 @@
       <c r="Q47" s="49"/>
       <c r="R47" s="49"/>
     </row>
-    <row r="48" spans="1:18" s="50" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" s="50" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A48" s="33" t="s">
         <v>208</v>
       </c>
@@ -8400,7 +8428,7 @@
       <c r="Q48" s="49"/>
       <c r="R48" s="49"/>
     </row>
-    <row r="49" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" s="50" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A49" s="33" t="s">
         <v>210</v>
       </c>
@@ -8426,7 +8454,7 @@
       <c r="Q49" s="49"/>
       <c r="R49" s="49"/>
     </row>
-    <row r="50" spans="1:18" s="50" customFormat="1" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" s="50" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A50" s="53" t="s">
         <v>212</v>
       </c>
@@ -8452,7 +8480,7 @@
       <c r="Q50" s="49"/>
       <c r="R50" s="49"/>
     </row>
-    <row r="51" spans="1:18" s="50" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" s="50" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A51" s="53" t="s">
         <v>214</v>
       </c>
@@ -8478,7 +8506,7 @@
       <c r="Q51" s="49"/>
       <c r="R51" s="49"/>
     </row>
-    <row r="52" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A52" s="53" t="s">
         <v>216</v>
       </c>
@@ -8504,7 +8532,7 @@
       <c r="Q52" s="49"/>
       <c r="R52" s="49"/>
     </row>
-    <row r="53" spans="1:18" s="50" customFormat="1" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" s="50" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A53" s="53" t="s">
         <v>218</v>
       </c>
@@ -8530,7 +8558,7 @@
       <c r="Q53" s="49"/>
       <c r="R53" s="49"/>
     </row>
-    <row r="54" spans="1:18" s="50" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" s="50" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A54" s="53" t="s">
         <v>220</v>
       </c>
@@ -8556,7 +8584,7 @@
       <c r="Q54" s="49"/>
       <c r="R54" s="49"/>
     </row>
-    <row r="55" spans="1:18" s="50" customFormat="1" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" s="50" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A55" s="53" t="s">
         <v>222</v>
       </c>
@@ -8582,7 +8610,7 @@
       <c r="Q55" s="49"/>
       <c r="R55" s="49"/>
     </row>
-    <row r="56" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A56" s="53" t="s">
         <v>224</v>
       </c>
@@ -8608,7 +8636,7 @@
       <c r="Q56" s="49"/>
       <c r="R56" s="49"/>
     </row>
-    <row r="57" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A57" s="53" t="s">
         <v>224</v>
       </c>
@@ -8634,7 +8662,7 @@
       <c r="Q57" s="49"/>
       <c r="R57" s="49"/>
     </row>
-    <row r="58" spans="1:18" s="50" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" s="50" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A58" s="53" t="s">
         <v>224</v>
       </c>
@@ -8660,7 +8688,7 @@
       <c r="Q58" s="49"/>
       <c r="R58" s="49"/>
     </row>
-    <row r="59" spans="1:18" s="50" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" s="50" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A59" s="53" t="s">
         <v>228</v>
       </c>
@@ -8686,7 +8714,7 @@
       <c r="Q59" s="49"/>
       <c r="R59" s="49"/>
     </row>
-    <row r="60" spans="1:18" s="50" customFormat="1" ht="81" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" s="50" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A60" s="53" t="s">
         <v>230</v>
       </c>
@@ -8712,7 +8740,7 @@
       <c r="Q60" s="49"/>
       <c r="R60" s="49"/>
     </row>
-    <row r="61" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A61" s="53" t="s">
         <v>228</v>
       </c>
@@ -8738,7 +8766,7 @@
       <c r="Q61" s="49"/>
       <c r="R61" s="49"/>
     </row>
-    <row r="62" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A62" s="53" t="s">
         <v>233</v>
       </c>
@@ -8764,7 +8792,7 @@
       <c r="Q62" s="49"/>
       <c r="R62" s="49"/>
     </row>
-    <row r="63" spans="1:18" s="50" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" s="50" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A63" s="53" t="s">
         <v>235</v>
       </c>
@@ -8790,7 +8818,7 @@
       <c r="Q63" s="49"/>
       <c r="R63" s="49"/>
     </row>
-    <row r="64" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A64" s="53" t="s">
         <v>237</v>
       </c>
@@ -8816,7 +8844,7 @@
       <c r="Q64" s="49"/>
       <c r="R64" s="49"/>
     </row>
-    <row r="65" spans="1:18" s="50" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:18" s="50" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="55" t="s">
         <v>239</v>
       </c>
@@ -8842,7 +8870,7 @@
       <c r="Q65" s="49"/>
       <c r="R65" s="49"/>
     </row>
-    <row r="66" spans="1:18" s="50" customFormat="1" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:18" s="50" customFormat="1" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="53" t="s">
         <v>241</v>
       </c>
@@ -8866,7 +8894,7 @@
       <c r="Q66" s="49"/>
       <c r="R66" s="49"/>
     </row>
-    <row r="67" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="14" t="s">
         <v>22</v>
       </c>
@@ -8891,7 +8919,7 @@
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
     </row>
-    <row r="68" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A68" s="16"/>
       <c r="B68" s="16"/>
       <c r="C68" s="16"/>
@@ -8911,7 +8939,7 @@
       <c r="Q68" s="4"/>
       <c r="R68" s="4"/>
     </row>
-    <row r="69" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
@@ -8961,7 +8989,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="71" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A71" s="19"/>
       <c r="B71" s="19"/>
       <c r="C71" s="20"/>
@@ -8981,7 +9009,7 @@
       <c r="Q71" s="4"/>
       <c r="R71" s="4"/>
     </row>
-    <row r="72" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="9"/>
@@ -9001,7 +9029,7 @@
       <c r="Q72" s="4"/>
       <c r="R72" s="4"/>
     </row>
-    <row r="73" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="9"/>
@@ -9021,7 +9049,7 @@
       <c r="Q73" s="4"/>
       <c r="R73" s="4"/>
     </row>
-    <row r="74" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="9"/>
@@ -9041,7 +9069,7 @@
       <c r="Q74" s="4"/>
       <c r="R74" s="4"/>
     </row>
-    <row r="75" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="9"/>
@@ -9061,7 +9089,7 @@
       <c r="Q75" s="4"/>
       <c r="R75" s="4"/>
     </row>
-    <row r="76" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="9"/>
@@ -9081,7 +9109,7 @@
       <c r="Q76" s="4"/>
       <c r="R76" s="4"/>
     </row>
-    <row r="77" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="25"/>
       <c r="B77" s="25"/>
       <c r="C77" s="26"/>
@@ -9101,7 +9129,7 @@
       <c r="Q77" s="4"/>
       <c r="R77" s="4"/>
     </row>
-    <row r="78" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="25"/>
       <c r="B78" s="25"/>
       <c r="C78" s="26"/>
@@ -9121,7 +9149,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="79" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="25"/>
       <c r="B79" s="25"/>
       <c r="C79" s="26"/>
@@ -9141,7 +9169,7 @@
       <c r="Q79" s="4"/>
       <c r="R79" s="4"/>
     </row>
-    <row r="80" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="25"/>
       <c r="B80" s="25"/>
       <c r="C80" s="26"/>
@@ -9161,7 +9189,7 @@
       <c r="Q80" s="4"/>
       <c r="R80" s="4"/>
     </row>
-    <row r="81" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="23"/>
       <c r="B81" s="23"/>
       <c r="C81" s="24"/>
@@ -9181,7 +9209,7 @@
       <c r="Q81" s="4"/>
       <c r="R81" s="4"/>
     </row>
-    <row r="82" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="14" t="s">
         <v>22</v>
       </c>
@@ -9206,7 +9234,7 @@
       <c r="Q82" s="4"/>
       <c r="R82" s="4"/>
     </row>
-    <row r="83" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="16"/>
       <c r="B83" s="16"/>
       <c r="C83" s="16"/>
@@ -9226,7 +9254,7 @@
       <c r="Q83" s="4"/>
       <c r="R83" s="4"/>
     </row>
-    <row r="84" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
@@ -9250,7 +9278,7 @@
       <c r="Q84" s="4"/>
       <c r="R84" s="4"/>
     </row>
-    <row r="85" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>2</v>
       </c>
@@ -9276,7 +9304,7 @@
       <c r="Q85" s="4"/>
       <c r="R85" s="4"/>
     </row>
-    <row r="86" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="19"/>
       <c r="B86" s="19"/>
       <c r="C86" s="20"/>
@@ -9296,7 +9324,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="87" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="9"/>
@@ -9316,7 +9344,7 @@
       <c r="Q87" s="4"/>
       <c r="R87" s="4"/>
     </row>
-    <row r="88" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="9"/>
@@ -9336,7 +9364,7 @@
       <c r="Q88" s="4"/>
       <c r="R88" s="4"/>
     </row>
-    <row r="89" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="9"/>
@@ -9356,7 +9384,7 @@
       <c r="Q89" s="4"/>
       <c r="R89" s="4"/>
     </row>
-    <row r="90" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="9"/>
@@ -9376,7 +9404,7 @@
       <c r="Q90" s="4"/>
       <c r="R90" s="4"/>
     </row>
-    <row r="91" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A91" s="23"/>
       <c r="B91" s="23"/>
       <c r="C91" s="24"/>
@@ -9396,7 +9424,7 @@
       <c r="Q91" s="4"/>
       <c r="R91" s="4"/>
     </row>
-    <row r="92" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A92" s="14" t="s">
         <v>22</v>
       </c>
@@ -9421,7 +9449,7 @@
       <c r="Q92" s="4"/>
       <c r="R92" s="4"/>
     </row>
-    <row r="93" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A93" s="16"/>
       <c r="B93" s="16"/>
       <c r="C93" s="16"/>
@@ -9441,7 +9469,7 @@
       <c r="Q93" s="4"/>
       <c r="R93" s="4"/>
     </row>
-    <row r="94" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>0</v>
       </c>
@@ -9491,7 +9519,7 @@
       <c r="Q95" s="4"/>
       <c r="R95" s="4"/>
     </row>
-    <row r="96" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A96" s="19"/>
       <c r="B96" s="19"/>
       <c r="C96" s="20"/>
@@ -9511,7 +9539,7 @@
       <c r="Q96" s="4"/>
       <c r="R96" s="4"/>
     </row>
-    <row r="97" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="9"/>
@@ -9531,7 +9559,7 @@
       <c r="Q97" s="4"/>
       <c r="R97" s="4"/>
     </row>
-    <row r="98" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="9"/>
@@ -9551,7 +9579,7 @@
       <c r="Q98" s="4"/>
       <c r="R98" s="4"/>
     </row>
-    <row r="99" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="9"/>
@@ -9571,7 +9599,7 @@
       <c r="Q99" s="4"/>
       <c r="R99" s="4"/>
     </row>
-    <row r="100" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="9"/>
@@ -9591,7 +9619,7 @@
       <c r="Q100" s="4"/>
       <c r="R100" s="4"/>
     </row>
-    <row r="101" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="9"/>
@@ -9611,7 +9639,7 @@
       <c r="Q101" s="4"/>
       <c r="R101" s="4"/>
     </row>
-    <row r="102" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="9"/>
@@ -9631,7 +9659,7 @@
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
     </row>
-    <row r="103" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A103" s="23"/>
       <c r="B103" s="23"/>
       <c r="C103" s="24"/>
@@ -9651,7 +9679,7 @@
       <c r="Q103" s="4"/>
       <c r="R103" s="4"/>
     </row>
-    <row r="104" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A104" s="14" t="s">
         <v>22</v>
       </c>
@@ -9676,7 +9704,7 @@
       <c r="Q104" s="4"/>
       <c r="R104" s="4"/>
     </row>
-    <row r="105" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A105" s="16"/>
       <c r="B105" s="16"/>
       <c r="C105" s="16"/>
@@ -9696,7 +9724,7 @@
       <c r="Q105" s="4"/>
       <c r="R105" s="4"/>
     </row>
-    <row r="106" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A106" s="27"/>
       <c r="B106" s="27"/>
       <c r="C106" s="27"/>
@@ -9716,7 +9744,7 @@
       <c r="Q106" s="4"/>
       <c r="R106" s="4"/>
     </row>
-    <row r="107" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A107" s="27"/>
       <c r="B107" s="27"/>
       <c r="C107" s="27"/>
@@ -9736,7 +9764,7 @@
       <c r="Q107" s="4"/>
       <c r="R107" s="4"/>
     </row>
-    <row r="108" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A108" s="27"/>
       <c r="B108" s="27"/>
       <c r="C108" s="27"/>
@@ -9756,7 +9784,7 @@
       <c r="Q108" s="4"/>
       <c r="R108" s="4"/>
     </row>
-    <row r="109" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A109" s="27"/>
       <c r="B109" s="27"/>
       <c r="C109" s="27"/>
@@ -9776,7 +9804,7 @@
       <c r="Q109" s="4"/>
       <c r="R109" s="4"/>
     </row>
-    <row r="110" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A110" s="27"/>
       <c r="B110" s="27"/>
       <c r="C110" s="27"/>
@@ -9796,7 +9824,7 @@
       <c r="Q110" s="4"/>
       <c r="R110" s="4"/>
     </row>
-    <row r="111" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A111" s="27"/>
       <c r="B111" s="27"/>
       <c r="C111" s="27"/>
@@ -9816,7 +9844,7 @@
       <c r="Q111" s="4"/>
       <c r="R111" s="4"/>
     </row>
-    <row r="112" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A112" s="27"/>
       <c r="B112" s="27"/>
       <c r="C112" s="27"/>
@@ -9836,7 +9864,7 @@
       <c r="Q112" s="4"/>
       <c r="R112" s="4"/>
     </row>
-    <row r="113" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A113" s="27"/>
       <c r="B113" s="27"/>
       <c r="C113" s="27"/>
@@ -9856,7 +9884,7 @@
       <c r="Q113" s="4"/>
       <c r="R113" s="4"/>
     </row>
-    <row r="114" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A114" s="27"/>
       <c r="B114" s="27"/>
       <c r="C114" s="27"/>
@@ -9876,7 +9904,7 @@
       <c r="Q114" s="4"/>
       <c r="R114" s="4"/>
     </row>
-    <row r="115" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A115" s="27"/>
       <c r="B115" s="27"/>
       <c r="C115" s="27"/>
@@ -9896,7 +9924,7 @@
       <c r="Q115" s="4"/>
       <c r="R115" s="4"/>
     </row>
-    <row r="116" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A116" s="27"/>
       <c r="B116" s="27"/>
       <c r="C116" s="27"/>
@@ -9916,7 +9944,7 @@
       <c r="Q116" s="4"/>
       <c r="R116" s="4"/>
     </row>
-    <row r="117" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A117" s="28"/>
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
@@ -9954,18 +9982,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F222774-5003-490D-9078-78D1F6F89A4A}">
   <dimension ref="A1:R100"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9991,7 +10019,7 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -10019,7 +10047,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -10047,7 +10075,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -10075,7 +10103,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -10103,7 +10131,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
@@ -10131,7 +10159,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>14</v>
       </c>
@@ -10159,7 +10187,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" ht="108" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>16</v>
       </c>
@@ -10187,7 +10215,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>18</v>
       </c>
@@ -10215,7 +10243,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
@@ -10243,7 +10271,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
@@ -10269,7 +10297,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
         <v>29</v>
       </c>
@@ -10295,7 +10323,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="33" t="s">
         <v>32</v>
       </c>
@@ -10321,7 +10349,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>22</v>
       </c>
@@ -10346,7 +10374,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -10366,7 +10394,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -10390,7 +10418,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>2</v>
       </c>
@@ -10416,7 +10444,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
         <v>36</v>
       </c>
@@ -10444,7 +10472,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>40</v>
       </c>
@@ -10472,7 +10500,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>54</v>
       </c>
@@ -10500,7 +10528,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -10528,7 +10556,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -10556,7 +10584,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>54</v>
       </c>
@@ -10584,7 +10612,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -10612,7 +10640,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>86</v>
       </c>
@@ -10640,7 +10668,7 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
     </row>
-    <row r="26" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>76</v>
       </c>
@@ -10668,7 +10696,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>76</v>
       </c>
@@ -10696,7 +10724,7 @@
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>76</v>
       </c>
@@ -10724,7 +10752,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>76</v>
       </c>
@@ -10752,7 +10780,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>76</v>
       </c>
@@ -10780,7 +10808,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="9"/>
@@ -10800,7 +10828,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="9"/>
@@ -10820,7 +10848,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="33" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="9"/>
@@ -10840,7 +10868,7 @@
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
     </row>
-    <row r="34" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
         <v>22</v>
       </c>
@@ -10865,7 +10893,7 @@
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -10885,7 +10913,7 @@
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -10909,7 +10937,7 @@
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
     </row>
-    <row r="37" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>2</v>
       </c>
@@ -10935,7 +10963,7 @@
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
     </row>
-    <row r="38" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>40</v>
       </c>
@@ -10963,7 +10991,7 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>160</v>
       </c>
@@ -10991,7 +11019,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="40" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>160</v>
       </c>
@@ -11019,7 +11047,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>160</v>
       </c>
@@ -11047,7 +11075,7 @@
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
     </row>
-    <row r="42" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>160</v>
       </c>
@@ -11075,7 +11103,7 @@
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>160</v>
       </c>
@@ -11103,7 +11131,7 @@
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
     </row>
-    <row r="44" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>160</v>
       </c>
@@ -11131,7 +11159,7 @@
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
     </row>
-    <row r="45" spans="1:18" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="23" t="s">
         <v>160</v>
       </c>
@@ -11159,7 +11187,7 @@
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
     </row>
-    <row r="46" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="42" t="s">
         <v>160</v>
       </c>
@@ -11187,7 +11215,7 @@
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
     </row>
-    <row r="47" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="42" t="s">
         <v>160</v>
       </c>
@@ -11215,7 +11243,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="48" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="42" t="s">
         <v>160</v>
       </c>
@@ -11243,7 +11271,7 @@
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
     </row>
-    <row r="49" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="42"/>
       <c r="B49" s="42"/>
       <c r="C49" s="44"/>
@@ -11263,7 +11291,7 @@
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
     </row>
-    <row r="50" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
         <v>22</v>
       </c>
@@ -11288,7 +11316,7 @@
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
     </row>
-    <row r="51" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="16"/>
       <c r="B51" s="16"/>
       <c r="C51" s="16"/>
@@ -11308,7 +11336,7 @@
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
     </row>
-    <row r="52" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -11332,7 +11360,7 @@
       <c r="Q52" s="4"/>
       <c r="R52" s="4"/>
     </row>
-    <row r="53" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>2</v>
       </c>
@@ -11358,7 +11386,7 @@
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
     </row>
-    <row r="54" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A54" s="19"/>
       <c r="B54" s="19"/>
       <c r="C54" s="20"/>
@@ -11378,7 +11406,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="55" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="9"/>
@@ -11398,7 +11426,7 @@
       <c r="Q55" s="4"/>
       <c r="R55" s="4"/>
     </row>
-    <row r="56" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="9"/>
@@ -11418,7 +11446,7 @@
       <c r="Q56" s="4"/>
       <c r="R56" s="4"/>
     </row>
-    <row r="57" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="9"/>
@@ -11438,7 +11466,7 @@
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
     </row>
-    <row r="58" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="9"/>
@@ -11458,7 +11486,7 @@
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
     </row>
-    <row r="59" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="9"/>
@@ -11478,7 +11506,7 @@
       <c r="Q59" s="4"/>
       <c r="R59" s="4"/>
     </row>
-    <row r="60" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A60" s="25"/>
       <c r="B60" s="25"/>
       <c r="C60" s="26"/>
@@ -11498,7 +11526,7 @@
       <c r="Q60" s="4"/>
       <c r="R60" s="4"/>
     </row>
-    <row r="61" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A61" s="25"/>
       <c r="B61" s="25"/>
       <c r="C61" s="26"/>
@@ -11518,7 +11546,7 @@
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
     </row>
-    <row r="62" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A62" s="25"/>
       <c r="B62" s="25"/>
       <c r="C62" s="26"/>
@@ -11538,7 +11566,7 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="63" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A63" s="25"/>
       <c r="B63" s="25"/>
       <c r="C63" s="26"/>
@@ -11558,7 +11586,7 @@
       <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
     </row>
-    <row r="64" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="23"/>
       <c r="B64" s="23"/>
       <c r="C64" s="24"/>
@@ -11578,7 +11606,7 @@
       <c r="Q64" s="4"/>
       <c r="R64" s="4"/>
     </row>
-    <row r="65" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="14" t="s">
         <v>22</v>
       </c>
@@ -11603,7 +11631,7 @@
       <c r="Q65" s="4"/>
       <c r="R65" s="4"/>
     </row>
-    <row r="66" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="16"/>
       <c r="B66" s="16"/>
       <c r="C66" s="16"/>
@@ -11623,7 +11651,7 @@
       <c r="Q66" s="4"/>
       <c r="R66" s="4"/>
     </row>
-    <row r="67" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -11647,7 +11675,7 @@
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
     </row>
-    <row r="68" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>2</v>
       </c>
@@ -11673,7 +11701,7 @@
       <c r="Q68" s="4"/>
       <c r="R68" s="4"/>
     </row>
-    <row r="69" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A69" s="19"/>
       <c r="B69" s="19"/>
       <c r="C69" s="20"/>
@@ -11693,7 +11721,7 @@
       <c r="Q69" s="4"/>
       <c r="R69" s="4"/>
     </row>
-    <row r="70" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="9"/>
@@ -11713,7 +11741,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="71" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="9"/>
@@ -11733,7 +11761,7 @@
       <c r="Q71" s="4"/>
       <c r="R71" s="4"/>
     </row>
-    <row r="72" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="9"/>
@@ -11753,7 +11781,7 @@
       <c r="Q72" s="4"/>
       <c r="R72" s="4"/>
     </row>
-    <row r="73" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="9"/>
@@ -11773,7 +11801,7 @@
       <c r="Q73" s="4"/>
       <c r="R73" s="4"/>
     </row>
-    <row r="74" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="23"/>
       <c r="B74" s="23"/>
       <c r="C74" s="24"/>
@@ -11793,7 +11821,7 @@
       <c r="Q74" s="4"/>
       <c r="R74" s="4"/>
     </row>
-    <row r="75" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
         <v>22</v>
       </c>
@@ -11818,7 +11846,7 @@
       <c r="Q75" s="4"/>
       <c r="R75" s="4"/>
     </row>
-    <row r="76" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="16"/>
       <c r="B76" s="16"/>
       <c r="C76" s="16"/>
@@ -11838,7 +11866,7 @@
       <c r="Q76" s="4"/>
       <c r="R76" s="4"/>
     </row>
-    <row r="77" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
@@ -11862,7 +11890,7 @@
       <c r="Q77" s="4"/>
       <c r="R77" s="4"/>
     </row>
-    <row r="78" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>2</v>
       </c>
@@ -11888,7 +11916,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="79" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A79" s="19"/>
       <c r="B79" s="19"/>
       <c r="C79" s="20"/>
@@ -11908,7 +11936,7 @@
       <c r="Q79" s="4"/>
       <c r="R79" s="4"/>
     </row>
-    <row r="80" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="9"/>
@@ -11928,7 +11956,7 @@
       <c r="Q80" s="4"/>
       <c r="R80" s="4"/>
     </row>
-    <row r="81" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="9"/>
@@ -11948,7 +11976,7 @@
       <c r="Q81" s="4"/>
       <c r="R81" s="4"/>
     </row>
-    <row r="82" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="9"/>
@@ -11968,7 +11996,7 @@
       <c r="Q82" s="4"/>
       <c r="R82" s="4"/>
     </row>
-    <row r="83" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="9"/>
@@ -11988,7 +12016,7 @@
       <c r="Q83" s="4"/>
       <c r="R83" s="4"/>
     </row>
-    <row r="84" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="9"/>
@@ -12008,7 +12036,7 @@
       <c r="Q84" s="4"/>
       <c r="R84" s="4"/>
     </row>
-    <row r="85" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="9"/>
@@ -12028,7 +12056,7 @@
       <c r="Q85" s="4"/>
       <c r="R85" s="4"/>
     </row>
-    <row r="86" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="23"/>
       <c r="B86" s="23"/>
       <c r="C86" s="24"/>
@@ -12048,7 +12076,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="87" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="14" t="s">
         <v>22</v>
       </c>
@@ -12073,7 +12101,7 @@
       <c r="Q87" s="4"/>
       <c r="R87" s="4"/>
     </row>
-    <row r="88" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A88" s="16"/>
       <c r="B88" s="16"/>
       <c r="C88" s="16"/>
@@ -12093,7 +12121,7 @@
       <c r="Q88" s="4"/>
       <c r="R88" s="4"/>
     </row>
-    <row r="89" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A89" s="27"/>
       <c r="B89" s="27"/>
       <c r="C89" s="27"/>
@@ -12113,7 +12141,7 @@
       <c r="Q89" s="4"/>
       <c r="R89" s="4"/>
     </row>
-    <row r="90" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A90" s="27"/>
       <c r="B90" s="27"/>
       <c r="C90" s="27"/>
@@ -12133,7 +12161,7 @@
       <c r="Q90" s="4"/>
       <c r="R90" s="4"/>
     </row>
-    <row r="91" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A91" s="27"/>
       <c r="B91" s="27"/>
       <c r="C91" s="27"/>
@@ -12153,7 +12181,7 @@
       <c r="Q91" s="4"/>
       <c r="R91" s="4"/>
     </row>
-    <row r="92" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A92" s="27"/>
       <c r="B92" s="27"/>
       <c r="C92" s="27"/>
@@ -12173,7 +12201,7 @@
       <c r="Q92" s="4"/>
       <c r="R92" s="4"/>
     </row>
-    <row r="93" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A93" s="27"/>
       <c r="B93" s="27"/>
       <c r="C93" s="27"/>
@@ -12193,7 +12221,7 @@
       <c r="Q93" s="4"/>
       <c r="R93" s="4"/>
     </row>
-    <row r="94" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A94" s="27"/>
       <c r="B94" s="27"/>
       <c r="C94" s="27"/>
@@ -12213,7 +12241,7 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="95" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A95" s="27"/>
       <c r="B95" s="27"/>
       <c r="C95" s="27"/>
@@ -12233,7 +12261,7 @@
       <c r="Q95" s="4"/>
       <c r="R95" s="4"/>
     </row>
-    <row r="96" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A96" s="27"/>
       <c r="B96" s="27"/>
       <c r="C96" s="27"/>
@@ -12253,7 +12281,7 @@
       <c r="Q96" s="4"/>
       <c r="R96" s="4"/>
     </row>
-    <row r="97" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A97" s="27"/>
       <c r="B97" s="27"/>
       <c r="C97" s="27"/>
@@ -12273,7 +12301,7 @@
       <c r="Q97" s="4"/>
       <c r="R97" s="4"/>
     </row>
-    <row r="98" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A98" s="27"/>
       <c r="B98" s="27"/>
       <c r="C98" s="27"/>
@@ -12293,7 +12321,7 @@
       <c r="Q98" s="4"/>
       <c r="R98" s="4"/>
     </row>
-    <row r="99" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A99" s="27"/>
       <c r="B99" s="27"/>
       <c r="C99" s="27"/>
@@ -12313,7 +12341,7 @@
       <c r="Q99" s="4"/>
       <c r="R99" s="4"/>
     </row>
-    <row r="100" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A100" s="28"/>
       <c r="B100" s="28"/>
       <c r="C100" s="28"/>
@@ -12346,4 +12374,511 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04752183-13CB-498C-B47A-4401EA9BDEF9}">
+  <dimension ref="A1:D65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.109375" customWidth="1"/>
+    <col min="4" max="4" width="46.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="B3" s="33">
+        <v>4</v>
+      </c>
+      <c r="C3" s="46">
+        <v>43969</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>254</v>
+      </c>
+      <c r="B4" s="33">
+        <v>4</v>
+      </c>
+      <c r="C4" s="46">
+        <v>43970</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" s="33">
+        <v>3</v>
+      </c>
+      <c r="C5" s="46">
+        <v>43976</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>255</v>
+      </c>
+      <c r="B6" s="33">
+        <v>1</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>256</v>
+      </c>
+      <c r="D6" s="51"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="53"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="53"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="53"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="53"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="53"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="54"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="53"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="53"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="53"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="53"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="53"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="53"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="53"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="53"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="53"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+    </row>
+    <row r="25" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="55"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+    </row>
+    <row r="26" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="53"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+    </row>
+    <row r="27" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+    </row>
+    <row r="28" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+    </row>
+    <row r="29" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="25"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="25"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+    </row>
+    <row r="41" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="23"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+    </row>
+    <row r="42" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="14">
+        <f>SUM(B31:B41)</f>
+        <v>0</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+    </row>
+    <row r="43" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+    </row>
+    <row r="44" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="2">
+        <v>5</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="19"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+    </row>
+    <row r="51" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="23"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+    </row>
+    <row r="52" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="14">
+        <f>SUM(B46:B51)</f>
+        <v>0</v>
+      </c>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+    </row>
+    <row r="53" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+    </row>
+    <row r="54" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="2">
+        <v>6</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="19"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="7"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+    </row>
+    <row r="63" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="23"/>
+      <c r="B63" s="23"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+    </row>
+    <row r="64" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B64" s="14">
+        <f>SUM(B56:B63)</f>
+        <v>0</v>
+      </c>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+    </row>
+    <row r="65" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A65" s="16"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B27 B42 B52 B64" xr:uid="{DA0CB379-8208-4014-8C0C-0521765B9A4F}">
+      <formula1>0</formula1>
+      <formula2>DureePeriode-1</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B56:B63 B31:B41 B46:B51 B3:B4 B6:B26" xr:uid="{FBF1D711-E5DD-4569-8B54-987F2C077F7C}">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update journal travail SEB + Equipe
</commit_message>
<xml_diff>
--- a/LM_Journal_Travail_V1.0.xlsx
+++ b/LM_Journal_Travail_V1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Love-Mirroring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35979477-834C-4A76-8BEA-AA658F52C99C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E4B803-2CD9-481E-8F9E-02C0A5131DA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="293">
   <si>
     <t>Jalon</t>
   </si>
@@ -958,6 +958,24 @@
   </si>
   <si>
     <t>J'ai modifié le contrôleur pour les publicités j'ai eu pas mal de souci pour traiter l'image que j'ai finalement converti en bytes et en base64 pour pouvoir la décoder dans l'API. Il me reste plus qu'à faire la fonction Edit et le Delete et afficher des pubs aléatoire sur la page de l'application.</t>
+  </si>
+  <si>
+    <t>J'affiche des publicités sur la page d'accueil avec un lien j'ai aussi regardé pour adapter l'EDIT et j'ai effectué quelques tests sur la plateforme en DEV. Monsieur Allemann va déployer ma version et je pourrais faire des tests en production.</t>
+  </si>
+  <si>
+    <t>Daily Scrum</t>
+  </si>
+  <si>
+    <t>3 semaines</t>
+  </si>
+  <si>
+    <t>Daily SCRUM régulier de l'équipe</t>
+  </si>
+  <si>
+    <t>Production + Test</t>
+  </si>
+  <si>
+    <t>Mise en production et test des fonctionnalités en équipe</t>
   </si>
 </sst>
 </file>
@@ -1673,8 +1691,8 @@
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2766,10 +2784,18 @@
       <c r="R47" s="4"/>
     </row>
     <row r="48" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="19"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
+      <c r="A48" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="B48" s="19">
+        <v>3.5</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>290</v>
+      </c>
       <c r="E48" s="10"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -2785,11 +2811,19 @@
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
     </row>
-    <row r="49" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
+    <row r="49" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="B49" s="7">
+        <v>4</v>
+      </c>
+      <c r="C49" s="35">
+        <v>43982</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>292</v>
+      </c>
       <c r="E49" s="10"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -2991,7 +3025,7 @@
       </c>
       <c r="B59" s="14">
         <f>SUM(B48:B58)</f>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="C59" s="15"/>
       <c r="D59" s="15"/>
@@ -4663,10 +4697,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB7A04D-A66F-4A89-83F1-9B353075A776}">
-  <dimension ref="A1:R107"/>
+  <dimension ref="A1:R108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -6611,16 +6645,19 @@
       <c r="Q71" s="4"/>
       <c r="R71" s="4"/>
     </row>
-    <row r="72" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B72" s="14">
-        <f>SUM(B60:B71)</f>
-        <v>39</v>
-      </c>
-      <c r="C72" s="15"/>
-      <c r="D72" s="15"/>
+    <row r="72" spans="1:18" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="42" t="s">
+        <v>285</v>
+      </c>
+      <c r="B72" s="42">
+        <v>4</v>
+      </c>
+      <c r="C72" s="43">
+        <v>43980</v>
+      </c>
+      <c r="D72" s="44" t="s">
+        <v>287</v>
+      </c>
       <c r="E72" s="10"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
@@ -6637,10 +6674,15 @@
       <c r="R72" s="4"/>
     </row>
     <row r="73" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="16"/>
-      <c r="B73" s="16"/>
-      <c r="C73" s="16"/>
-      <c r="D73" s="16"/>
+      <c r="A73" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B73" s="14">
+        <f>SUM(B60:B72)</f>
+        <v>43</v>
+      </c>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
       <c r="E73" s="10"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
@@ -6656,15 +6698,11 @@
       <c r="Q73" s="4"/>
       <c r="R73" s="4"/>
     </row>
-    <row r="74" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B74" s="2">
-        <v>5</v>
-      </c>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
+    <row r="74" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="16"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
       <c r="E74" s="10"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
@@ -6680,17 +6718,15 @@
       <c r="Q74" s="4"/>
       <c r="R74" s="4"/>
     </row>
-    <row r="75" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5" t="s">
+    <row r="75" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="2">
         <v>5</v>
       </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
       <c r="E75" s="10"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
@@ -6706,11 +6742,17 @@
       <c r="Q75" s="4"/>
       <c r="R75" s="4"/>
     </row>
-    <row r="76" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A76" s="19"/>
-      <c r="B76" s="19"/>
-      <c r="C76" s="20"/>
-      <c r="D76" s="20"/>
+    <row r="76" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E76" s="10"/>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
@@ -6727,10 +6769,10 @@
       <c r="R76" s="4"/>
     </row>
     <row r="77" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A77" s="7"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="9"/>
-      <c r="D77" s="9"/>
+      <c r="A77" s="19"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="20"/>
+      <c r="D77" s="20"/>
       <c r="E77" s="10"/>
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
@@ -6806,11 +6848,11 @@
       <c r="Q80" s="4"/>
       <c r="R80" s="4"/>
     </row>
-    <row r="81" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="23"/>
-      <c r="B81" s="23"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
+    <row r="81" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
       <c r="E81" s="10"/>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
@@ -6827,15 +6869,10 @@
       <c r="R81" s="4"/>
     </row>
     <row r="82" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B82" s="14">
-        <f>SUM(B76:B81)</f>
-        <v>0</v>
-      </c>
-      <c r="C82" s="15"/>
-      <c r="D82" s="15"/>
+      <c r="A82" s="23"/>
+      <c r="B82" s="23"/>
+      <c r="C82" s="24"/>
+      <c r="D82" s="24"/>
       <c r="E82" s="10"/>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
@@ -6852,10 +6889,15 @@
       <c r="R82" s="4"/>
     </row>
     <row r="83" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="16"/>
-      <c r="B83" s="16"/>
-      <c r="C83" s="16"/>
-      <c r="D83" s="16"/>
+      <c r="A83" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B83" s="14">
+        <f>SUM(B77:B82)</f>
+        <v>0</v>
+      </c>
+      <c r="C83" s="15"/>
+      <c r="D83" s="15"/>
       <c r="E83" s="10"/>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
@@ -6871,15 +6913,11 @@
       <c r="Q83" s="4"/>
       <c r="R83" s="4"/>
     </row>
-    <row r="84" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B84" s="2">
-        <v>6</v>
-      </c>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
+    <row r="84" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="16"/>
+      <c r="B84" s="16"/>
+      <c r="C84" s="16"/>
+      <c r="D84" s="16"/>
       <c r="E84" s="10"/>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
@@ -6895,17 +6933,15 @@
       <c r="Q84" s="4"/>
       <c r="R84" s="4"/>
     </row>
-    <row r="85" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5" t="s">
-        <v>5</v>
-      </c>
+    <row r="85" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B85" s="2">
+        <v>6</v>
+      </c>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
       <c r="E85" s="10"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
@@ -6921,11 +6957,17 @@
       <c r="Q85" s="4"/>
       <c r="R85" s="4"/>
     </row>
-    <row r="86" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A86" s="19"/>
-      <c r="B86" s="19"/>
-      <c r="C86" s="20"/>
-      <c r="D86" s="20"/>
+    <row r="86" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E86" s="10"/>
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
@@ -6942,10 +6984,10 @@
       <c r="R86" s="4"/>
     </row>
     <row r="87" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A87" s="7"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="9"/>
-      <c r="D87" s="9"/>
+      <c r="A87" s="19"/>
+      <c r="B87" s="19"/>
+      <c r="C87" s="20"/>
+      <c r="D87" s="20"/>
       <c r="E87" s="10"/>
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
@@ -7061,11 +7103,11 @@
       <c r="Q92" s="4"/>
       <c r="R92" s="4"/>
     </row>
-    <row r="93" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="23"/>
-      <c r="B93" s="23"/>
-      <c r="C93" s="24"/>
-      <c r="D93" s="24"/>
+    <row r="93" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A93" s="7"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
       <c r="E93" s="10"/>
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
@@ -7082,15 +7124,10 @@
       <c r="R93" s="4"/>
     </row>
     <row r="94" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B94" s="14">
-        <f>SUM(B86:B93)</f>
-        <v>0</v>
-      </c>
-      <c r="C94" s="15"/>
-      <c r="D94" s="15"/>
+      <c r="A94" s="23"/>
+      <c r="B94" s="23"/>
+      <c r="C94" s="24"/>
+      <c r="D94" s="24"/>
       <c r="E94" s="10"/>
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
@@ -7106,11 +7143,16 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="95" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A95" s="16"/>
-      <c r="B95" s="16"/>
-      <c r="C95" s="16"/>
-      <c r="D95" s="16"/>
+    <row r="95" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B95" s="14">
+        <f>SUM(B87:B94)</f>
+        <v>0</v>
+      </c>
+      <c r="C95" s="15"/>
+      <c r="D95" s="15"/>
       <c r="E95" s="10"/>
       <c r="F95" s="4"/>
       <c r="G95" s="4"/>
@@ -7127,10 +7169,10 @@
       <c r="R95" s="4"/>
     </row>
     <row r="96" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A96" s="27"/>
-      <c r="B96" s="27"/>
-      <c r="C96" s="27"/>
-      <c r="D96" s="27"/>
+      <c r="A96" s="16"/>
+      <c r="B96" s="16"/>
+      <c r="C96" s="16"/>
+      <c r="D96" s="16"/>
       <c r="E96" s="10"/>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
@@ -7331,20 +7373,40 @@
       <c r="B106" s="27"/>
       <c r="C106" s="27"/>
       <c r="D106" s="27"/>
+      <c r="E106" s="10"/>
+      <c r="F106" s="4"/>
+      <c r="G106" s="4"/>
+      <c r="H106" s="4"/>
+      <c r="I106" s="4"/>
+      <c r="J106" s="4"/>
+      <c r="K106" s="4"/>
+      <c r="L106" s="4"/>
+      <c r="M106" s="4"/>
+      <c r="N106" s="4"/>
+      <c r="O106" s="4"/>
+      <c r="P106" s="4"/>
+      <c r="Q106" s="4"/>
+      <c r="R106" s="4"/>
     </row>
     <row r="107" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A107" s="28"/>
-      <c r="B107" s="28"/>
-      <c r="C107" s="28"/>
-      <c r="D107" s="28"/>
+      <c r="A107" s="27"/>
+      <c r="B107" s="27"/>
+      <c r="C107" s="27"/>
+      <c r="D107" s="27"/>
+    </row>
+    <row r="108" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+      <c r="A108" s="28"/>
+      <c r="B108" s="28"/>
+      <c r="C108" s="28"/>
+      <c r="D108" s="28"/>
     </row>
   </sheetData>
   <dataValidations xWindow="188" yWindow="522" count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B12 B34 B56 B72 B82 B94" xr:uid="{41F29EDA-D509-4469-8DFB-6A4CE4CEAE07}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B12 B34 B56 B73 B83 B95" xr:uid="{41F29EDA-D509-4469-8DFB-6A4CE4CEAE07}">
       <formula1>0</formula1>
       <formula2>DureePeriode-1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B86:B93 B38:B39 B41:B45 B76:B81 B10:B11 B3:B8 B16:B33 B60:B71" xr:uid="{3039B7E3-952E-4B34-B612-E5A0C049619C}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B87:B94 B38:B39 B41:B45 B77:B82 B10:B11 B3:B8 B16:B33 B60:B72" xr:uid="{3039B7E3-952E-4B34-B612-E5A0C049619C}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
recup des documents de test
</commit_message>
<xml_diff>
--- a/LM_Journal_Travail_V1.0.xlsx
+++ b/LM_Journal_Travail_V1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Documents\GitHub\Love-Mirroring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA5C19A-794A-4D38-BDFD-879283793BA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D71629-CD07-479F-A6DC-EC2CCF92FFC0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="271">
   <si>
     <t>Jalon</t>
   </si>
@@ -858,21 +858,66 @@
     <t>Modification interface administration -Commencement CRUD Sexes</t>
   </si>
   <si>
-    <t>Modification interface administration - CRUD Sexualités</t>
-  </si>
-  <si>
-    <t>25,05,20</t>
+    <t>Affichage, création, modification, 
+suppression des sexualités</t>
+  </si>
+  <si>
+    <t>Recherche pour les demandes de contact</t>
+  </si>
+  <si>
+    <t>Demandes de contact</t>
+  </si>
+  <si>
+    <t>Création de l'interface et modification du script SQL afin d'ajouter des tables dans la BD</t>
+  </si>
+  <si>
+    <t>Modification interface administration - interface Sexualités</t>
+  </si>
+  <si>
+    <t>interface Corpulences</t>
+  </si>
+  <si>
+    <t>interface Religions</t>
+  </si>
+  <si>
+    <t>interface Styles</t>
+  </si>
+  <si>
+    <t>interface Questions</t>
+  </si>
+  <si>
+    <t>interface Profils</t>
+  </si>
+  <si>
+    <t>interface Reponses</t>
+  </si>
+  <si>
+    <t>interface Cheveux tailles</t>
+  </si>
+  <si>
+    <t>interface Cheveux couleurs</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>Affichage de toutes les réponses d'une demande de contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procédure de test
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
     <numFmt numFmtId="165" formatCode="dd\.mm\.yy"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -929,6 +974,12 @@
     </font>
     <font>
       <sz val="9"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
       <family val="2"/>
@@ -1186,7 +1237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1353,6 +1404,45 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4566,7 +4656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB7A04D-A66F-4A89-83F1-9B353075A776}">
   <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
@@ -7185,8 +7275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716E2DDB-6361-470B-ACF3-8FDF9046203A}">
   <dimension ref="A1:R117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9982,8 +10072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F222774-5003-490D-9078-78D1F6F89A4A}">
   <dimension ref="A1:R100"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -12378,10 +12468,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04752183-13CB-498C-B47A-4401EA9BDEF9}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -12456,101 +12546,153 @@
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="B6" s="33">
+        <v>2</v>
+      </c>
+      <c r="C6" s="61">
+        <v>43976</v>
+      </c>
+      <c r="D6" s="51" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="33">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="B7" s="68">
+        <v>6</v>
+      </c>
+      <c r="C7" s="65">
+        <v>43977</v>
+      </c>
+      <c r="D7" s="71" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>261</v>
+      </c>
+      <c r="B8" s="69"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="72"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="B9" s="69"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="72"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="53" t="s">
+        <v>263</v>
+      </c>
+      <c r="B10" s="69"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="72"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="53" t="s">
+        <v>264</v>
+      </c>
+      <c r="B11" s="69"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="72"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="B12" s="69"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="72"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="62" t="s">
+        <v>266</v>
+      </c>
+      <c r="B13" s="69"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="72"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="62" t="s">
+        <v>267</v>
+      </c>
+      <c r="B14" s="70"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="73"/>
+    </row>
+    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="53" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15" s="53">
         <v>1</v>
       </c>
-      <c r="C6" s="51" t="s">
-        <v>256</v>
-      </c>
-      <c r="D6" s="51"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
-      <c r="B15" s="53"/>
-      <c r="C15" s="54"/>
+      <c r="C15" s="67"/>
       <c r="D15" s="54"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="68" t="s">
+        <v>257</v>
+      </c>
+      <c r="B16" s="63">
+        <v>2.5</v>
+      </c>
+      <c r="C16" s="64">
+        <v>43978</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="54"/>
+      <c r="A17" s="69"/>
+      <c r="B17" s="53">
+        <v>4</v>
+      </c>
+      <c r="C17" s="64">
+        <v>43979</v>
+      </c>
       <c r="D17" s="54"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
+    <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="69"/>
+      <c r="B18" s="53">
+        <v>4</v>
+      </c>
+      <c r="C18" s="64">
+        <v>43980</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
+      <c r="A19" s="70"/>
       <c r="B19" s="53"/>
-      <c r="C19" s="54"/>
+      <c r="C19" s="64">
+        <v>43982</v>
+      </c>
       <c r="D19" s="54"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="53"/>
       <c r="B20" s="53"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
+      <c r="C20" s="64">
+        <v>43982</v>
+      </c>
+      <c r="D20" s="54" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="53"/>
@@ -12576,71 +12718,74 @@
       <c r="C24" s="54"/>
       <c r="D24" s="54"/>
     </row>
-    <row r="25" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="55"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-    </row>
-    <row r="26" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="53"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="53"/>
       <c r="B26" s="53"/>
       <c r="C26" s="54"/>
       <c r="D26" s="54"/>
     </row>
     <row r="27" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="55"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+    </row>
+    <row r="28" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="53"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+    </row>
+    <row r="29" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-    </row>
-    <row r="28" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-    </row>
-    <row r="29" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="B29" s="14">
+        <f>SUM(B3:B27)</f>
+        <v>30.5</v>
+      </c>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+    </row>
+    <row r="30" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+    </row>
+    <row r="31" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B31" s="2">
         <v>4</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5" t="s">
+      <c r="C32" s="5"/>
+      <c r="D32" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-    </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
@@ -12661,16 +12806,16 @@
       <c r="D36" s="9"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="25"/>
@@ -12684,68 +12829,68 @@
       <c r="C40" s="26"/>
       <c r="D40" s="26"/>
     </row>
-    <row r="41" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="23"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-    </row>
-    <row r="42" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="14" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="25"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="25"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+    </row>
+    <row r="43" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+    </row>
+    <row r="44" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="14">
-        <f>SUM(B31:B41)</f>
+      <c r="B44" s="14">
+        <f>SUM(B33:B43)</f>
         <v>0</v>
       </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-    </row>
-    <row r="43" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-    </row>
-    <row r="44" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+    </row>
+    <row r="45" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+    </row>
+    <row r="46" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B46" s="2">
         <v>5</v>
       </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B47" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5" t="s">
+      <c r="C47" s="5"/>
+      <c r="D47" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-    </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
+      <c r="A48" s="19"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
@@ -12759,68 +12904,68 @@
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
     </row>
-    <row r="51" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="23"/>
-      <c r="B51" s="23"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-    </row>
-    <row r="52" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="14" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+    </row>
+    <row r="53" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="23"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+    </row>
+    <row r="54" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B52" s="14">
-        <f>SUM(B46:B51)</f>
+      <c r="B54" s="14">
+        <f>SUM(B48:B53)</f>
         <v>0</v>
       </c>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-    </row>
-    <row r="53" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="16"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-    </row>
-    <row r="54" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+    </row>
+    <row r="55" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="16"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+    </row>
+    <row r="56" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B56" s="2">
         <v>6</v>
       </c>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-    </row>
-    <row r="55" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B57" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5" t="s">
+      <c r="C57" s="5"/>
+      <c r="D57" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="19"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-    </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
+      <c r="A58" s="19"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
@@ -12846,39 +12991,58 @@
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
     </row>
-    <row r="63" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="23"/>
-      <c r="B63" s="23"/>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
-    </row>
-    <row r="64" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="14" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+    </row>
+    <row r="65" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="23"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="24"/>
+      <c r="D65" s="24"/>
+    </row>
+    <row r="66" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B64" s="14">
-        <f>SUM(B56:B63)</f>
+      <c r="B66" s="14">
+        <f>SUM(B58:B65)</f>
         <v>0</v>
       </c>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
-    </row>
-    <row r="65" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A65" s="16"/>
-      <c r="B65" s="16"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+    </row>
+    <row r="67" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A67" s="16"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C7:C15"/>
+    <mergeCell ref="B7:B14"/>
+    <mergeCell ref="D7:D14"/>
+    <mergeCell ref="A16:A19"/>
+  </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B27 B42 B52 B64" xr:uid="{DA0CB379-8208-4014-8C0C-0521765B9A4F}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B29 B44 B54 B66" xr:uid="{DA0CB379-8208-4014-8C0C-0521765B9A4F}">
       <formula1>0</formula1>
       <formula2>DureePeriode-1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B56:B63 B31:B41 B46:B51 B3:B4 B6:B26" xr:uid="{FBF1D711-E5DD-4569-8B54-987F2C077F7C}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B58:B65 B33:B43 B48:B53 B3:B4 B6:B7 B15:B28" xr:uid="{FBF1D711-E5DD-4569-8B54-987F2C077F7C}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test Paul + maj journal de travail
</commit_message>
<xml_diff>
--- a/LM_Journal_Travail_V1.0.xlsx
+++ b/LM_Journal_Travail_V1.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Love-Mirroring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Documents\GitHub\Love-Mirroring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410FC245-90E6-4E1F-87F6-923DCE4B17F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74AA46D-B5CF-4B78-A143-9B3FDE4A3E32}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="317">
   <si>
     <t>Jalon</t>
   </si>
@@ -901,13 +901,6 @@
     <t>"</t>
   </si>
   <si>
-    <t>Affichage de toutes les réponses d'une demande de contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Procédure de test
-</t>
-  </si>
-  <si>
     <t>Daily Scrum</t>
   </si>
   <si>
@@ -1054,6 +1047,16 @@
   </si>
   <si>
     <t>Test + Correction</t>
+  </si>
+  <si>
+    <t>Côté admin: Affichage de toutes les réponses d'une demande de contact</t>
+  </si>
+  <si>
+    <t>Côté utilisateur: affichage des demandes de contact de l'utilisateur connecté</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procédure de test: quand je veux voir les réponses, je ne peux voir que le texte et la valeur de la réponse, il manque l'affichage du profil et de la question.
+</t>
   </si>
 </sst>
 </file>
@@ -1385,7 +1388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1568,6 +1571,12 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1594,6 +1603,16 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1819,16 +1838,16 @@
       <selection activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="78.42578125" customWidth="1"/>
-    <col min="5" max="6" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="78.44140625" customWidth="1"/>
+    <col min="5" max="6" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1854,7 +1873,7 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -1882,7 +1901,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -1910,7 +1929,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -1938,7 +1957,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -1966,7 +1985,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
@@ -1994,7 +2013,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>14</v>
       </c>
@@ -2022,7 +2041,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>16</v>
       </c>
@@ -2050,7 +2069,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>18</v>
       </c>
@@ -2078,7 +2097,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
@@ -2106,7 +2125,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
@@ -2126,7 +2145,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>22</v>
       </c>
@@ -2151,7 +2170,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -2171,7 +2190,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -2195,7 +2214,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>2</v>
       </c>
@@ -2221,7 +2240,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
         <v>95</v>
       </c>
@@ -2249,7 +2268,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>99</v>
       </c>
@@ -2277,7 +2296,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="9"/>
@@ -2297,7 +2316,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="9"/>
@@ -2317,7 +2336,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="9"/>
@@ -2909,16 +2928,16 @@
     </row>
     <row r="48" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="19" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B48" s="19">
         <v>3.5</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E48" s="10"/>
       <c r="F48" s="4"/>
@@ -2935,9 +2954,9 @@
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
     </row>
-    <row r="49" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B49" s="7">
         <v>4</v>
@@ -2946,7 +2965,7 @@
         <v>43982</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E49" s="10"/>
       <c r="F49" s="4"/>
@@ -4823,18 +4842,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB7A04D-A66F-4A89-83F1-9B353075A776}">
   <dimension ref="A1:R110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4860,7 +4879,7 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -4888,7 +4907,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -4916,7 +4935,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -4944,7 +4963,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -4972,7 +4991,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
@@ -5000,7 +5019,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>14</v>
       </c>
@@ -5028,7 +5047,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>16</v>
       </c>
@@ -5056,7 +5075,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>18</v>
       </c>
@@ -5084,7 +5103,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
@@ -5112,7 +5131,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
@@ -5140,7 +5159,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>22</v>
       </c>
@@ -5165,7 +5184,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -5185,7 +5204,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -5209,7 +5228,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>2</v>
       </c>
@@ -5235,7 +5254,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>36</v>
       </c>
@@ -5263,7 +5282,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>38</v>
       </c>
@@ -5291,7 +5310,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>42</v>
       </c>
@@ -5319,7 +5338,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
@@ -5347,7 +5366,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>46</v>
       </c>
@@ -5375,7 +5394,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>48</v>
       </c>
@@ -5403,7 +5422,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>50</v>
       </c>
@@ -5431,7 +5450,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18" ht="121.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>73</v>
       </c>
@@ -5459,7 +5478,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>52</v>
       </c>
@@ -5487,7 +5506,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>62</v>
       </c>
@@ -5515,7 +5534,7 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
     </row>
-    <row r="26" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>63</v>
       </c>
@@ -5543,7 +5562,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>65</v>
       </c>
@@ -5571,7 +5590,7 @@
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>69</v>
       </c>
@@ -5599,7 +5618,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>71</v>
       </c>
@@ -5627,7 +5646,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>88</v>
       </c>
@@ -5655,7 +5674,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>90</v>
       </c>
@@ -5683,7 +5702,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A32" s="38" t="s">
         <v>97</v>
       </c>
@@ -5711,7 +5730,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="33" spans="1:18" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="38" t="s">
         <v>142</v>
       </c>
@@ -5739,7 +5758,7 @@
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
     </row>
-    <row r="34" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
         <v>22</v>
       </c>
@@ -5764,7 +5783,7 @@
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -5784,7 +5803,7 @@
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -5808,7 +5827,7 @@
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
     </row>
-    <row r="37" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>2</v>
       </c>
@@ -5834,7 +5853,7 @@
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
     </row>
-    <row r="38" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>148</v>
       </c>
@@ -5862,7 +5881,7 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>150</v>
       </c>
@@ -5890,7 +5909,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="40" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>152</v>
       </c>
@@ -5918,7 +5937,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>154</v>
       </c>
@@ -5946,7 +5965,7 @@
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
     </row>
-    <row r="42" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>156</v>
       </c>
@@ -5974,7 +5993,7 @@
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>158</v>
       </c>
@@ -6002,7 +6021,7 @@
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
     </row>
-    <row r="44" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>165</v>
       </c>
@@ -6030,7 +6049,7 @@
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
     </row>
-    <row r="45" spans="1:18" ht="81.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="23" t="s">
         <v>167</v>
       </c>
@@ -6058,7 +6077,7 @@
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
     </row>
-    <row r="46" spans="1:18" ht="108.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" ht="106.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="23" t="s">
         <v>169</v>
       </c>
@@ -6086,7 +6105,7 @@
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
     </row>
-    <row r="47" spans="1:18" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="42" t="s">
         <v>171</v>
       </c>
@@ -6114,7 +6133,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="48" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="42" t="s">
         <v>173</v>
       </c>
@@ -6142,7 +6161,7 @@
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
     </row>
-    <row r="49" spans="1:18" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="42" t="s">
         <v>181</v>
       </c>
@@ -6170,7 +6189,7 @@
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
     </row>
-    <row r="50" spans="1:18" ht="81.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:18" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="42" t="s">
         <v>183</v>
       </c>
@@ -6198,7 +6217,7 @@
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
     </row>
-    <row r="51" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="42" t="s">
         <v>189</v>
       </c>
@@ -6226,7 +6245,7 @@
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
     </row>
-    <row r="52" spans="1:18" ht="68.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:18" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="42" t="s">
         <v>191</v>
       </c>
@@ -6254,7 +6273,7 @@
       <c r="Q52" s="4"/>
       <c r="R52" s="4"/>
     </row>
-    <row r="53" spans="1:18" ht="81.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="42" t="s">
         <v>195</v>
       </c>
@@ -6282,7 +6301,7 @@
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
     </row>
-    <row r="54" spans="1:18" ht="81.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="42" t="s">
         <v>197</v>
       </c>
@@ -6310,7 +6329,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="55" spans="1:18" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:18" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="42" t="s">
         <v>243</v>
       </c>
@@ -6338,7 +6357,7 @@
       <c r="Q55" s="4"/>
       <c r="R55" s="4"/>
     </row>
-    <row r="56" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="14" t="s">
         <v>22</v>
       </c>
@@ -6363,7 +6382,7 @@
       <c r="Q56" s="4"/>
       <c r="R56" s="4"/>
     </row>
-    <row r="57" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="16"/>
       <c r="B57" s="16"/>
       <c r="C57" s="16"/>
@@ -6383,7 +6402,7 @@
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
     </row>
-    <row r="58" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
@@ -6407,7 +6426,7 @@
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
     </row>
-    <row r="59" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>2</v>
       </c>
@@ -6433,7 +6452,7 @@
       <c r="Q59" s="4"/>
       <c r="R59" s="4"/>
     </row>
-    <row r="60" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A60" s="19" t="s">
         <v>245</v>
       </c>
@@ -6461,7 +6480,7 @@
       <c r="Q60" s="4"/>
       <c r="R60" s="4"/>
     </row>
-    <row r="61" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A61" s="58" t="s">
         <v>245</v>
       </c>
@@ -6489,7 +6508,7 @@
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
     </row>
-    <row r="62" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>245</v>
       </c>
@@ -6517,7 +6536,7 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="63" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>245</v>
       </c>
@@ -6528,7 +6547,7 @@
         <v>43969</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E63" s="10"/>
       <c r="F63" s="4"/>
@@ -6545,9 +6564,9 @@
       <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
     </row>
-    <row r="64" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B64" s="7">
         <v>5.5</v>
@@ -6556,7 +6575,7 @@
         <v>43970</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E64" s="10"/>
       <c r="F64" s="4"/>
@@ -6573,9 +6592,9 @@
       <c r="Q64" s="4"/>
       <c r="R64" s="4"/>
     </row>
-    <row r="65" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B65" s="7">
         <v>3.5</v>
@@ -6584,7 +6603,7 @@
         <v>43971</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E65" s="10"/>
       <c r="F65" s="4"/>
@@ -6601,9 +6620,9 @@
       <c r="Q65" s="4"/>
       <c r="R65" s="4"/>
     </row>
-    <row r="66" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B66" s="7">
         <v>1.5</v>
@@ -6612,7 +6631,7 @@
         <v>43972</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E66" s="10"/>
       <c r="F66" s="4"/>
@@ -6629,7 +6648,7 @@
       <c r="Q66" s="4"/>
       <c r="R66" s="4"/>
     </row>
-    <row r="67" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A67" s="25" t="s">
         <v>183</v>
       </c>
@@ -6640,7 +6659,7 @@
         <v>43974</v>
       </c>
       <c r="D67" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E67" s="10"/>
       <c r="F67" s="4"/>
@@ -6657,7 +6676,7 @@
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
     </row>
-    <row r="68" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A68" s="25" t="s">
         <v>183</v>
       </c>
@@ -6668,7 +6687,7 @@
         <v>43975</v>
       </c>
       <c r="D68" s="26" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E68" s="10"/>
       <c r="F68" s="4"/>
@@ -6685,9 +6704,9 @@
       <c r="Q68" s="4"/>
       <c r="R68" s="4"/>
     </row>
-    <row r="69" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A69" s="25" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B69" s="25">
         <v>4</v>
@@ -6696,7 +6715,7 @@
         <v>43976</v>
       </c>
       <c r="D69" s="26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E69" s="10"/>
       <c r="F69" s="4"/>
@@ -6713,9 +6732,9 @@
       <c r="Q69" s="4"/>
       <c r="R69" s="4"/>
     </row>
-    <row r="70" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A70" s="25" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B70" s="25">
         <v>4.5</v>
@@ -6724,7 +6743,7 @@
         <v>43977</v>
       </c>
       <c r="D70" s="26" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E70" s="10"/>
       <c r="F70" s="4"/>
@@ -6741,9 +6760,9 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="71" spans="1:18" ht="54.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:18" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="23" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B71" s="23">
         <v>4</v>
@@ -6752,7 +6771,7 @@
         <v>43979</v>
       </c>
       <c r="D71" s="24" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E71" s="10"/>
       <c r="F71" s="4"/>
@@ -6769,9 +6788,9 @@
       <c r="Q71" s="4"/>
       <c r="R71" s="4"/>
     </row>
-    <row r="72" spans="1:18" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:18" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="42" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B72" s="42">
         <v>4</v>
@@ -6780,7 +6799,7 @@
         <v>43980</v>
       </c>
       <c r="D72" s="44" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E72" s="10"/>
       <c r="F72" s="4"/>
@@ -6797,7 +6816,7 @@
       <c r="Q72" s="4"/>
       <c r="R72" s="4"/>
     </row>
-    <row r="73" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="42" t="s">
         <v>235</v>
       </c>
@@ -6808,7 +6827,7 @@
         <v>43981</v>
       </c>
       <c r="D73" s="44" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E73" s="10"/>
       <c r="F73" s="4"/>
@@ -6825,9 +6844,9 @@
       <c r="Q73" s="4"/>
       <c r="R73" s="4"/>
     </row>
-    <row r="74" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="42" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B74" s="42"/>
       <c r="C74" s="43"/>
@@ -6847,7 +6866,7 @@
       <c r="Q74" s="4"/>
       <c r="R74" s="4"/>
     </row>
-    <row r="75" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
         <v>22</v>
       </c>
@@ -6872,7 +6891,7 @@
       <c r="Q75" s="4"/>
       <c r="R75" s="4"/>
     </row>
-    <row r="76" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="16"/>
       <c r="B76" s="16"/>
       <c r="C76" s="16"/>
@@ -6892,7 +6911,7 @@
       <c r="Q76" s="4"/>
       <c r="R76" s="4"/>
     </row>
-    <row r="77" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
@@ -6916,7 +6935,7 @@
       <c r="Q77" s="4"/>
       <c r="R77" s="4"/>
     </row>
-    <row r="78" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>2</v>
       </c>
@@ -6942,7 +6961,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="79" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A79" s="19"/>
       <c r="B79" s="19"/>
       <c r="C79" s="20"/>
@@ -6962,7 +6981,7 @@
       <c r="Q79" s="4"/>
       <c r="R79" s="4"/>
     </row>
-    <row r="80" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="9"/>
@@ -6982,7 +7001,7 @@
       <c r="Q80" s="4"/>
       <c r="R80" s="4"/>
     </row>
-    <row r="81" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="9"/>
@@ -7002,7 +7021,7 @@
       <c r="Q81" s="4"/>
       <c r="R81" s="4"/>
     </row>
-    <row r="82" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="9"/>
@@ -7022,7 +7041,7 @@
       <c r="Q82" s="4"/>
       <c r="R82" s="4"/>
     </row>
-    <row r="83" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="9"/>
@@ -7042,7 +7061,7 @@
       <c r="Q83" s="4"/>
       <c r="R83" s="4"/>
     </row>
-    <row r="84" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="23"/>
       <c r="B84" s="23"/>
       <c r="C84" s="24"/>
@@ -7062,7 +7081,7 @@
       <c r="Q84" s="4"/>
       <c r="R84" s="4"/>
     </row>
-    <row r="85" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="14" t="s">
         <v>22</v>
       </c>
@@ -7087,7 +7106,7 @@
       <c r="Q85" s="4"/>
       <c r="R85" s="4"/>
     </row>
-    <row r="86" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="16"/>
       <c r="B86" s="16"/>
       <c r="C86" s="16"/>
@@ -7107,7 +7126,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="87" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>0</v>
       </c>
@@ -7131,7 +7150,7 @@
       <c r="Q87" s="4"/>
       <c r="R87" s="4"/>
     </row>
-    <row r="88" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>2</v>
       </c>
@@ -7157,7 +7176,7 @@
       <c r="Q88" s="4"/>
       <c r="R88" s="4"/>
     </row>
-    <row r="89" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A89" s="19"/>
       <c r="B89" s="19"/>
       <c r="C89" s="20"/>
@@ -7177,7 +7196,7 @@
       <c r="Q89" s="4"/>
       <c r="R89" s="4"/>
     </row>
-    <row r="90" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="9"/>
@@ -7197,7 +7216,7 @@
       <c r="Q90" s="4"/>
       <c r="R90" s="4"/>
     </row>
-    <row r="91" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="9"/>
@@ -7217,7 +7236,7 @@
       <c r="Q91" s="4"/>
       <c r="R91" s="4"/>
     </row>
-    <row r="92" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="9"/>
@@ -7237,7 +7256,7 @@
       <c r="Q92" s="4"/>
       <c r="R92" s="4"/>
     </row>
-    <row r="93" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="9"/>
@@ -7257,7 +7276,7 @@
       <c r="Q93" s="4"/>
       <c r="R93" s="4"/>
     </row>
-    <row r="94" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="9"/>
@@ -7277,7 +7296,7 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="95" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="9"/>
@@ -7297,7 +7316,7 @@
       <c r="Q95" s="4"/>
       <c r="R95" s="4"/>
     </row>
-    <row r="96" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="23"/>
       <c r="B96" s="23"/>
       <c r="C96" s="24"/>
@@ -7317,7 +7336,7 @@
       <c r="Q96" s="4"/>
       <c r="R96" s="4"/>
     </row>
-    <row r="97" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="14" t="s">
         <v>22</v>
       </c>
@@ -7342,7 +7361,7 @@
       <c r="Q97" s="4"/>
       <c r="R97" s="4"/>
     </row>
-    <row r="98" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A98" s="16"/>
       <c r="B98" s="16"/>
       <c r="C98" s="16"/>
@@ -7362,7 +7381,7 @@
       <c r="Q98" s="4"/>
       <c r="R98" s="4"/>
     </row>
-    <row r="99" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A99" s="27"/>
       <c r="B99" s="27"/>
       <c r="C99" s="27"/>
@@ -7382,7 +7401,7 @@
       <c r="Q99" s="4"/>
       <c r="R99" s="4"/>
     </row>
-    <row r="100" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A100" s="27"/>
       <c r="B100" s="27"/>
       <c r="C100" s="27"/>
@@ -7402,7 +7421,7 @@
       <c r="Q100" s="4"/>
       <c r="R100" s="4"/>
     </row>
-    <row r="101" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A101" s="27"/>
       <c r="B101" s="27"/>
       <c r="C101" s="27"/>
@@ -7422,7 +7441,7 @@
       <c r="Q101" s="4"/>
       <c r="R101" s="4"/>
     </row>
-    <row r="102" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A102" s="27"/>
       <c r="B102" s="27"/>
       <c r="C102" s="27"/>
@@ -7442,7 +7461,7 @@
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
     </row>
-    <row r="103" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A103" s="27"/>
       <c r="B103" s="27"/>
       <c r="C103" s="27"/>
@@ -7462,7 +7481,7 @@
       <c r="Q103" s="4"/>
       <c r="R103" s="4"/>
     </row>
-    <row r="104" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A104" s="27"/>
       <c r="B104" s="27"/>
       <c r="C104" s="27"/>
@@ -7482,7 +7501,7 @@
       <c r="Q104" s="4"/>
       <c r="R104" s="4"/>
     </row>
-    <row r="105" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A105" s="27"/>
       <c r="B105" s="27"/>
       <c r="C105" s="27"/>
@@ -7502,7 +7521,7 @@
       <c r="Q105" s="4"/>
       <c r="R105" s="4"/>
     </row>
-    <row r="106" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A106" s="27"/>
       <c r="B106" s="27"/>
       <c r="C106" s="27"/>
@@ -7522,7 +7541,7 @@
       <c r="Q106" s="4"/>
       <c r="R106" s="4"/>
     </row>
-    <row r="107" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A107" s="27"/>
       <c r="B107" s="27"/>
       <c r="C107" s="27"/>
@@ -7542,7 +7561,7 @@
       <c r="Q107" s="4"/>
       <c r="R107" s="4"/>
     </row>
-    <row r="108" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A108" s="27"/>
       <c r="B108" s="27"/>
       <c r="C108" s="27"/>
@@ -7562,13 +7581,13 @@
       <c r="Q108" s="4"/>
       <c r="R108" s="4"/>
     </row>
-    <row r="109" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A109" s="27"/>
       <c r="B109" s="27"/>
       <c r="C109" s="27"/>
       <c r="D109" s="27"/>
     </row>
-    <row r="110" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A110" s="28"/>
       <c r="B110" s="28"/>
       <c r="C110" s="28"/>
@@ -7593,18 +7612,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716E2DDB-6361-470B-ACF3-8FDF9046203A}">
   <dimension ref="A1:R117"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7630,7 +7649,7 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -7658,7 +7677,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -7686,7 +7705,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -7714,7 +7733,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -7742,7 +7761,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
@@ -7770,7 +7789,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>14</v>
       </c>
@@ -7798,7 +7817,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" ht="108" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>16</v>
       </c>
@@ -7826,7 +7845,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>18</v>
       </c>
@@ -7854,7 +7873,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
@@ -7882,7 +7901,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
@@ -7908,7 +7927,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -7934,7 +7953,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>22</v>
       </c>
@@ -7959,7 +7978,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -7979,7 +7998,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -8029,7 +8048,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>103</v>
       </c>
@@ -8055,7 +8074,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>105</v>
       </c>
@@ -8079,7 +8098,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>106</v>
       </c>
@@ -8105,7 +8124,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>108</v>
       </c>
@@ -8131,7 +8150,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>110</v>
       </c>
@@ -8157,7 +8176,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>112</v>
       </c>
@@ -8183,7 +8202,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>114</v>
       </c>
@@ -8209,7 +8228,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="1:18" ht="108" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>116</v>
       </c>
@@ -8235,7 +8254,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>118</v>
       </c>
@@ -8261,7 +8280,7 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
     </row>
-    <row r="26" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>120</v>
       </c>
@@ -8287,7 +8306,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" ht="121.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>122</v>
       </c>
@@ -8313,7 +8332,7 @@
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>124</v>
       </c>
@@ -8339,7 +8358,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>126</v>
       </c>
@@ -8365,7 +8384,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>124</v>
       </c>
@@ -8391,7 +8410,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>129</v>
       </c>
@@ -8417,7 +8436,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>131</v>
       </c>
@@ -8443,7 +8462,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="33" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>133</v>
       </c>
@@ -8469,7 +8488,7 @@
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
     </row>
-    <row r="34" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>134</v>
       </c>
@@ -8495,7 +8514,7 @@
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>136</v>
       </c>
@@ -8521,7 +8540,7 @@
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>138</v>
       </c>
@@ -8547,7 +8566,7 @@
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
     </row>
-    <row r="37" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>140</v>
       </c>
@@ -8573,7 +8592,7 @@
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
     </row>
-    <row r="38" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="9"/>
@@ -8593,7 +8612,7 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="14" t="s">
         <v>22</v>
       </c>
@@ -8618,7 +8637,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="40" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -8638,7 +8657,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -8662,7 +8681,7 @@
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
     </row>
-    <row r="42" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>2</v>
       </c>
@@ -8688,7 +8707,7 @@
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="1:18" s="50" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" s="50" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A43" s="33" t="s">
         <v>202</v>
       </c>
@@ -8712,7 +8731,7 @@
       <c r="Q43" s="49"/>
       <c r="R43" s="49"/>
     </row>
-    <row r="44" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A44" s="33" t="s">
         <v>203</v>
       </c>
@@ -8738,7 +8757,7 @@
       <c r="Q44" s="49"/>
       <c r="R44" s="49"/>
     </row>
-    <row r="45" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A45" s="33" t="s">
         <v>205</v>
       </c>
@@ -8762,7 +8781,7 @@
       <c r="Q45" s="49"/>
       <c r="R45" s="49"/>
     </row>
-    <row r="46" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A46" s="33" t="s">
         <v>206</v>
       </c>
@@ -8786,7 +8805,7 @@
       <c r="Q46" s="49"/>
       <c r="R46" s="49"/>
     </row>
-    <row r="47" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A47" s="33" t="s">
         <v>207</v>
       </c>
@@ -8810,7 +8829,7 @@
       <c r="Q47" s="49"/>
       <c r="R47" s="49"/>
     </row>
-    <row r="48" spans="1:18" s="50" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" s="50" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A48" s="33" t="s">
         <v>208</v>
       </c>
@@ -8836,7 +8855,7 @@
       <c r="Q48" s="49"/>
       <c r="R48" s="49"/>
     </row>
-    <row r="49" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" s="50" customFormat="1" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A49" s="33" t="s">
         <v>210</v>
       </c>
@@ -8862,7 +8881,7 @@
       <c r="Q49" s="49"/>
       <c r="R49" s="49"/>
     </row>
-    <row r="50" spans="1:18" s="50" customFormat="1" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" s="50" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A50" s="53" t="s">
         <v>212</v>
       </c>
@@ -8888,7 +8907,7 @@
       <c r="Q50" s="49"/>
       <c r="R50" s="49"/>
     </row>
-    <row r="51" spans="1:18" s="50" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" s="50" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A51" s="53" t="s">
         <v>214</v>
       </c>
@@ -8914,7 +8933,7 @@
       <c r="Q51" s="49"/>
       <c r="R51" s="49"/>
     </row>
-    <row r="52" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A52" s="53" t="s">
         <v>216</v>
       </c>
@@ -8940,7 +8959,7 @@
       <c r="Q52" s="49"/>
       <c r="R52" s="49"/>
     </row>
-    <row r="53" spans="1:18" s="50" customFormat="1" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" s="50" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A53" s="53" t="s">
         <v>218</v>
       </c>
@@ -8966,7 +8985,7 @@
       <c r="Q53" s="49"/>
       <c r="R53" s="49"/>
     </row>
-    <row r="54" spans="1:18" s="50" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" s="50" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A54" s="53" t="s">
         <v>220</v>
       </c>
@@ -8992,7 +9011,7 @@
       <c r="Q54" s="49"/>
       <c r="R54" s="49"/>
     </row>
-    <row r="55" spans="1:18" s="50" customFormat="1" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" s="50" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A55" s="53" t="s">
         <v>222</v>
       </c>
@@ -9018,7 +9037,7 @@
       <c r="Q55" s="49"/>
       <c r="R55" s="49"/>
     </row>
-    <row r="56" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A56" s="53" t="s">
         <v>224</v>
       </c>
@@ -9044,7 +9063,7 @@
       <c r="Q56" s="49"/>
       <c r="R56" s="49"/>
     </row>
-    <row r="57" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A57" s="53" t="s">
         <v>224</v>
       </c>
@@ -9070,7 +9089,7 @@
       <c r="Q57" s="49"/>
       <c r="R57" s="49"/>
     </row>
-    <row r="58" spans="1:18" s="50" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" s="50" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A58" s="53" t="s">
         <v>224</v>
       </c>
@@ -9096,7 +9115,7 @@
       <c r="Q58" s="49"/>
       <c r="R58" s="49"/>
     </row>
-    <row r="59" spans="1:18" s="50" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" s="50" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A59" s="53" t="s">
         <v>228</v>
       </c>
@@ -9122,7 +9141,7 @@
       <c r="Q59" s="49"/>
       <c r="R59" s="49"/>
     </row>
-    <row r="60" spans="1:18" s="50" customFormat="1" ht="81" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" s="50" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A60" s="53" t="s">
         <v>230</v>
       </c>
@@ -9148,7 +9167,7 @@
       <c r="Q60" s="49"/>
       <c r="R60" s="49"/>
     </row>
-    <row r="61" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A61" s="53" t="s">
         <v>228</v>
       </c>
@@ -9174,7 +9193,7 @@
       <c r="Q61" s="49"/>
       <c r="R61" s="49"/>
     </row>
-    <row r="62" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A62" s="53" t="s">
         <v>233</v>
       </c>
@@ -9200,7 +9219,7 @@
       <c r="Q62" s="49"/>
       <c r="R62" s="49"/>
     </row>
-    <row r="63" spans="1:18" s="50" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" s="50" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A63" s="53" t="s">
         <v>235</v>
       </c>
@@ -9226,7 +9245,7 @@
       <c r="Q63" s="49"/>
       <c r="R63" s="49"/>
     </row>
-    <row r="64" spans="1:18" s="50" customFormat="1" ht="27" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A64" s="53" t="s">
         <v>237</v>
       </c>
@@ -9252,7 +9271,7 @@
       <c r="Q64" s="49"/>
       <c r="R64" s="49"/>
     </row>
-    <row r="65" spans="1:18" s="50" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:18" s="50" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="55" t="s">
         <v>239</v>
       </c>
@@ -9278,7 +9297,7 @@
       <c r="Q65" s="49"/>
       <c r="R65" s="49"/>
     </row>
-    <row r="66" spans="1:18" s="50" customFormat="1" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:18" s="50" customFormat="1" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="53" t="s">
         <v>241</v>
       </c>
@@ -9302,7 +9321,7 @@
       <c r="Q66" s="49"/>
       <c r="R66" s="49"/>
     </row>
-    <row r="67" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="14" t="s">
         <v>22</v>
       </c>
@@ -9327,7 +9346,7 @@
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
     </row>
-    <row r="68" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A68" s="16"/>
       <c r="B68" s="16"/>
       <c r="C68" s="16"/>
@@ -9347,7 +9366,7 @@
       <c r="Q68" s="4"/>
       <c r="R68" s="4"/>
     </row>
-    <row r="69" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>0</v>
       </c>
@@ -9397,7 +9416,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="71" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A71" s="19"/>
       <c r="B71" s="19"/>
       <c r="C71" s="20"/>
@@ -9417,7 +9436,7 @@
       <c r="Q71" s="4"/>
       <c r="R71" s="4"/>
     </row>
-    <row r="72" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="9"/>
@@ -9437,7 +9456,7 @@
       <c r="Q72" s="4"/>
       <c r="R72" s="4"/>
     </row>
-    <row r="73" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="9"/>
@@ -9457,7 +9476,7 @@
       <c r="Q73" s="4"/>
       <c r="R73" s="4"/>
     </row>
-    <row r="74" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="9"/>
@@ -9477,7 +9496,7 @@
       <c r="Q74" s="4"/>
       <c r="R74" s="4"/>
     </row>
-    <row r="75" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="9"/>
@@ -9497,7 +9516,7 @@
       <c r="Q75" s="4"/>
       <c r="R75" s="4"/>
     </row>
-    <row r="76" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="9"/>
@@ -9517,7 +9536,7 @@
       <c r="Q76" s="4"/>
       <c r="R76" s="4"/>
     </row>
-    <row r="77" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="25"/>
       <c r="B77" s="25"/>
       <c r="C77" s="26"/>
@@ -9537,7 +9556,7 @@
       <c r="Q77" s="4"/>
       <c r="R77" s="4"/>
     </row>
-    <row r="78" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="25"/>
       <c r="B78" s="25"/>
       <c r="C78" s="26"/>
@@ -9557,7 +9576,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="79" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="25"/>
       <c r="B79" s="25"/>
       <c r="C79" s="26"/>
@@ -9577,7 +9596,7 @@
       <c r="Q79" s="4"/>
       <c r="R79" s="4"/>
     </row>
-    <row r="80" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="25"/>
       <c r="B80" s="25"/>
       <c r="C80" s="26"/>
@@ -9597,7 +9616,7 @@
       <c r="Q80" s="4"/>
       <c r="R80" s="4"/>
     </row>
-    <row r="81" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="23"/>
       <c r="B81" s="23"/>
       <c r="C81" s="24"/>
@@ -9617,7 +9636,7 @@
       <c r="Q81" s="4"/>
       <c r="R81" s="4"/>
     </row>
-    <row r="82" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="14" t="s">
         <v>22</v>
       </c>
@@ -9642,7 +9661,7 @@
       <c r="Q82" s="4"/>
       <c r="R82" s="4"/>
     </row>
-    <row r="83" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="16"/>
       <c r="B83" s="16"/>
       <c r="C83" s="16"/>
@@ -9662,7 +9681,7 @@
       <c r="Q83" s="4"/>
       <c r="R83" s="4"/>
     </row>
-    <row r="84" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>0</v>
       </c>
@@ -9686,7 +9705,7 @@
       <c r="Q84" s="4"/>
       <c r="R84" s="4"/>
     </row>
-    <row r="85" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>2</v>
       </c>
@@ -9712,7 +9731,7 @@
       <c r="Q85" s="4"/>
       <c r="R85" s="4"/>
     </row>
-    <row r="86" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="19"/>
       <c r="B86" s="19"/>
       <c r="C86" s="20"/>
@@ -9732,7 +9751,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="87" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="9"/>
@@ -9752,7 +9771,7 @@
       <c r="Q87" s="4"/>
       <c r="R87" s="4"/>
     </row>
-    <row r="88" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="9"/>
@@ -9772,7 +9791,7 @@
       <c r="Q88" s="4"/>
       <c r="R88" s="4"/>
     </row>
-    <row r="89" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="9"/>
@@ -9792,7 +9811,7 @@
       <c r="Q89" s="4"/>
       <c r="R89" s="4"/>
     </row>
-    <row r="90" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="9"/>
@@ -9812,7 +9831,7 @@
       <c r="Q90" s="4"/>
       <c r="R90" s="4"/>
     </row>
-    <row r="91" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A91" s="23"/>
       <c r="B91" s="23"/>
       <c r="C91" s="24"/>
@@ -9832,7 +9851,7 @@
       <c r="Q91" s="4"/>
       <c r="R91" s="4"/>
     </row>
-    <row r="92" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A92" s="14" t="s">
         <v>22</v>
       </c>
@@ -9857,7 +9876,7 @@
       <c r="Q92" s="4"/>
       <c r="R92" s="4"/>
     </row>
-    <row r="93" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A93" s="16"/>
       <c r="B93" s="16"/>
       <c r="C93" s="16"/>
@@ -9877,7 +9896,7 @@
       <c r="Q93" s="4"/>
       <c r="R93" s="4"/>
     </row>
-    <row r="94" spans="1:18" ht="18" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>0</v>
       </c>
@@ -9927,7 +9946,7 @@
       <c r="Q95" s="4"/>
       <c r="R95" s="4"/>
     </row>
-    <row r="96" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A96" s="19"/>
       <c r="B96" s="19"/>
       <c r="C96" s="20"/>
@@ -9947,7 +9966,7 @@
       <c r="Q96" s="4"/>
       <c r="R96" s="4"/>
     </row>
-    <row r="97" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="9"/>
@@ -9967,7 +9986,7 @@
       <c r="Q97" s="4"/>
       <c r="R97" s="4"/>
     </row>
-    <row r="98" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="9"/>
@@ -9987,7 +10006,7 @@
       <c r="Q98" s="4"/>
       <c r="R98" s="4"/>
     </row>
-    <row r="99" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="9"/>
@@ -10007,7 +10026,7 @@
       <c r="Q99" s="4"/>
       <c r="R99" s="4"/>
     </row>
-    <row r="100" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="9"/>
@@ -10027,7 +10046,7 @@
       <c r="Q100" s="4"/>
       <c r="R100" s="4"/>
     </row>
-    <row r="101" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="9"/>
@@ -10047,7 +10066,7 @@
       <c r="Q101" s="4"/>
       <c r="R101" s="4"/>
     </row>
-    <row r="102" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="9"/>
@@ -10067,7 +10086,7 @@
       <c r="Q102" s="4"/>
       <c r="R102" s="4"/>
     </row>
-    <row r="103" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A103" s="23"/>
       <c r="B103" s="23"/>
       <c r="C103" s="24"/>
@@ -10087,7 +10106,7 @@
       <c r="Q103" s="4"/>
       <c r="R103" s="4"/>
     </row>
-    <row r="104" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A104" s="14" t="s">
         <v>22</v>
       </c>
@@ -10112,7 +10131,7 @@
       <c r="Q104" s="4"/>
       <c r="R104" s="4"/>
     </row>
-    <row r="105" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A105" s="16"/>
       <c r="B105" s="16"/>
       <c r="C105" s="16"/>
@@ -10132,7 +10151,7 @@
       <c r="Q105" s="4"/>
       <c r="R105" s="4"/>
     </row>
-    <row r="106" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A106" s="27"/>
       <c r="B106" s="27"/>
       <c r="C106" s="27"/>
@@ -10152,7 +10171,7 @@
       <c r="Q106" s="4"/>
       <c r="R106" s="4"/>
     </row>
-    <row r="107" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A107" s="27"/>
       <c r="B107" s="27"/>
       <c r="C107" s="27"/>
@@ -10172,7 +10191,7 @@
       <c r="Q107" s="4"/>
       <c r="R107" s="4"/>
     </row>
-    <row r="108" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A108" s="27"/>
       <c r="B108" s="27"/>
       <c r="C108" s="27"/>
@@ -10192,7 +10211,7 @@
       <c r="Q108" s="4"/>
       <c r="R108" s="4"/>
     </row>
-    <row r="109" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A109" s="27"/>
       <c r="B109" s="27"/>
       <c r="C109" s="27"/>
@@ -10212,7 +10231,7 @@
       <c r="Q109" s="4"/>
       <c r="R109" s="4"/>
     </row>
-    <row r="110" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A110" s="27"/>
       <c r="B110" s="27"/>
       <c r="C110" s="27"/>
@@ -10232,7 +10251,7 @@
       <c r="Q110" s="4"/>
       <c r="R110" s="4"/>
     </row>
-    <row r="111" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A111" s="27"/>
       <c r="B111" s="27"/>
       <c r="C111" s="27"/>
@@ -10252,7 +10271,7 @@
       <c r="Q111" s="4"/>
       <c r="R111" s="4"/>
     </row>
-    <row r="112" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A112" s="27"/>
       <c r="B112" s="27"/>
       <c r="C112" s="27"/>
@@ -10272,7 +10291,7 @@
       <c r="Q112" s="4"/>
       <c r="R112" s="4"/>
     </row>
-    <row r="113" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A113" s="27"/>
       <c r="B113" s="27"/>
       <c r="C113" s="27"/>
@@ -10292,7 +10311,7 @@
       <c r="Q113" s="4"/>
       <c r="R113" s="4"/>
     </row>
-    <row r="114" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A114" s="27"/>
       <c r="B114" s="27"/>
       <c r="C114" s="27"/>
@@ -10312,7 +10331,7 @@
       <c r="Q114" s="4"/>
       <c r="R114" s="4"/>
     </row>
-    <row r="115" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A115" s="27"/>
       <c r="B115" s="27"/>
       <c r="C115" s="27"/>
@@ -10332,7 +10351,7 @@
       <c r="Q115" s="4"/>
       <c r="R115" s="4"/>
     </row>
-    <row r="116" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A116" s="27"/>
       <c r="B116" s="27"/>
       <c r="C116" s="27"/>
@@ -10352,7 +10371,7 @@
       <c r="Q116" s="4"/>
       <c r="R116" s="4"/>
     </row>
-    <row r="117" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A117" s="28"/>
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
@@ -10390,18 +10409,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F222774-5003-490D-9078-78D1F6F89A4A}">
   <dimension ref="A1:R100"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10427,7 +10446,7 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -10455,7 +10474,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
@@ -10483,7 +10502,7 @@
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
     </row>
-    <row r="4" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -10511,7 +10530,7 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
-    <row r="5" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -10539,7 +10558,7 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
     </row>
-    <row r="6" spans="1:18" ht="81" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
@@ -10567,7 +10586,7 @@
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
-    <row r="7" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>14</v>
       </c>
@@ -10595,7 +10614,7 @@
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
     </row>
-    <row r="8" spans="1:18" ht="108" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
         <v>16</v>
       </c>
@@ -10623,7 +10642,7 @@
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
     </row>
-    <row r="9" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
         <v>18</v>
       </c>
@@ -10651,7 +10670,7 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
     </row>
-    <row r="10" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>20</v>
       </c>
@@ -10679,7 +10698,7 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
     </row>
-    <row r="11" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
@@ -10705,7 +10724,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
     </row>
-    <row r="12" spans="1:18" ht="94.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A12" s="33" t="s">
         <v>29</v>
       </c>
@@ -10731,7 +10750,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
     </row>
-    <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="33" t="s">
         <v>32</v>
       </c>
@@ -10757,7 +10776,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
     </row>
-    <row r="14" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>22</v>
       </c>
@@ -10782,7 +10801,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
     </row>
-    <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -10802,7 +10821,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
     </row>
-    <row r="16" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -10826,7 +10845,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>2</v>
       </c>
@@ -10852,7 +10871,7 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
     </row>
-    <row r="18" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
         <v>36</v>
       </c>
@@ -10880,7 +10899,7 @@
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
     </row>
-    <row r="19" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>40</v>
       </c>
@@ -10908,7 +10927,7 @@
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
     </row>
-    <row r="20" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>54</v>
       </c>
@@ -10936,7 +10955,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -10964,7 +10983,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>58</v>
       </c>
@@ -10992,7 +11011,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>54</v>
       </c>
@@ -11020,7 +11039,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>60</v>
       </c>
@@ -11048,7 +11067,7 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>86</v>
       </c>
@@ -11076,7 +11095,7 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
     </row>
-    <row r="26" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>76</v>
       </c>
@@ -11104,7 +11123,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>76</v>
       </c>
@@ -11132,7 +11151,7 @@
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>76</v>
       </c>
@@ -11160,7 +11179,7 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>76</v>
       </c>
@@ -11188,7 +11207,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>76</v>
       </c>
@@ -11216,7 +11235,7 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="9"/>
@@ -11236,7 +11255,7 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="9"/>
@@ -11256,7 +11275,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="33" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="9"/>
@@ -11276,7 +11295,7 @@
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
     </row>
-    <row r="34" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
         <v>22</v>
       </c>
@@ -11301,7 +11320,7 @@
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -11321,7 +11340,7 @@
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>0</v>
       </c>
@@ -11345,7 +11364,7 @@
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
     </row>
-    <row r="37" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>2</v>
       </c>
@@ -11371,7 +11390,7 @@
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
     </row>
-    <row r="38" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>40</v>
       </c>
@@ -11399,7 +11418,7 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>160</v>
       </c>
@@ -11427,7 +11446,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="40" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>160</v>
       </c>
@@ -11455,7 +11474,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>160</v>
       </c>
@@ -11483,7 +11502,7 @@
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
     </row>
-    <row r="42" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>160</v>
       </c>
@@ -11511,7 +11530,7 @@
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>160</v>
       </c>
@@ -11539,7 +11558,7 @@
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
     </row>
-    <row r="44" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>160</v>
       </c>
@@ -11567,7 +11586,7 @@
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
     </row>
-    <row r="45" spans="1:18" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="23" t="s">
         <v>160</v>
       </c>
@@ -11595,7 +11614,7 @@
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
     </row>
-    <row r="46" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="42" t="s">
         <v>160</v>
       </c>
@@ -11623,7 +11642,7 @@
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
     </row>
-    <row r="47" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="42" t="s">
         <v>160</v>
       </c>
@@ -11651,7 +11670,7 @@
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
     </row>
-    <row r="48" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="42" t="s">
         <v>160</v>
       </c>
@@ -11679,7 +11698,7 @@
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
     </row>
-    <row r="49" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="42"/>
       <c r="B49" s="42"/>
       <c r="C49" s="44"/>
@@ -11699,7 +11718,7 @@
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
     </row>
-    <row r="50" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
         <v>22</v>
       </c>
@@ -11724,7 +11743,7 @@
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
     </row>
-    <row r="51" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="16"/>
       <c r="B51" s="16"/>
       <c r="C51" s="16"/>
@@ -11744,7 +11763,7 @@
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
     </row>
-    <row r="52" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -11768,7 +11787,7 @@
       <c r="Q52" s="4"/>
       <c r="R52" s="4"/>
     </row>
-    <row r="53" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>2</v>
       </c>
@@ -11794,7 +11813,7 @@
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
     </row>
-    <row r="54" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A54" s="19" t="s">
         <v>160</v>
       </c>
@@ -11802,10 +11821,10 @@
         <v>4</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E54" s="10"/>
       <c r="F54" s="4"/>
@@ -11822,7 +11841,7 @@
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
     </row>
-    <row r="55" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>160</v>
       </c>
@@ -11830,10 +11849,10 @@
         <v>4.5</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E55" s="10"/>
       <c r="F55" s="4"/>
@@ -11850,7 +11869,7 @@
       <c r="Q55" s="4"/>
       <c r="R55" s="4"/>
     </row>
-    <row r="56" spans="1:18" ht="54" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>160</v>
       </c>
@@ -11858,10 +11877,10 @@
         <v>3</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E56" s="10"/>
       <c r="F56" s="4"/>
@@ -11878,18 +11897,18 @@
       <c r="Q56" s="4"/>
       <c r="R56" s="4"/>
     </row>
-    <row r="57" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B57" s="7">
         <v>1.5</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E57" s="10"/>
       <c r="F57" s="4"/>
@@ -11906,18 +11925,18 @@
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
     </row>
-    <row r="58" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B58" s="7">
         <v>4</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E58" s="10"/>
       <c r="F58" s="4"/>
@@ -11934,18 +11953,18 @@
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
     </row>
-    <row r="59" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B59" s="7">
         <v>8</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E59" s="10"/>
       <c r="F59" s="4"/>
@@ -11962,18 +11981,18 @@
       <c r="Q59" s="4"/>
       <c r="R59" s="4"/>
     </row>
-    <row r="60" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A60" s="25" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B60" s="25">
         <v>5</v>
       </c>
       <c r="C60" s="26" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D60" s="26" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E60" s="10"/>
       <c r="F60" s="4"/>
@@ -11990,18 +12009,18 @@
       <c r="Q60" s="4"/>
       <c r="R60" s="4"/>
     </row>
-    <row r="61" spans="1:18" ht="27" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A61" s="25" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B61" s="25">
         <v>3</v>
       </c>
       <c r="C61" s="26" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D61" s="26" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E61" s="10"/>
       <c r="F61" s="4"/>
@@ -12018,18 +12037,18 @@
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
     </row>
-    <row r="62" spans="1:18" ht="40.5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A62" s="25" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B62" s="25">
         <v>3</v>
       </c>
       <c r="C62" s="26" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D62" s="26" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E62" s="10"/>
       <c r="F62" s="4"/>
@@ -12046,18 +12065,18 @@
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
     </row>
-    <row r="63" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:18" ht="66" x14ac:dyDescent="0.3">
       <c r="A63" s="25" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B63" s="25">
         <v>3</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D63" s="26" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E63" s="10"/>
       <c r="F63" s="4"/>
@@ -12074,18 +12093,18 @@
       <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
     </row>
-    <row r="64" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="23" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B64" s="23">
         <v>4</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D64" s="24" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E64" s="10"/>
       <c r="F64" s="4"/>
@@ -12102,7 +12121,7 @@
       <c r="Q64" s="4"/>
       <c r="R64" s="4"/>
     </row>
-    <row r="65" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="14" t="s">
         <v>22</v>
       </c>
@@ -12127,7 +12146,7 @@
       <c r="Q65" s="4"/>
       <c r="R65" s="4"/>
     </row>
-    <row r="66" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="16"/>
       <c r="B66" s="16"/>
       <c r="C66" s="16"/>
@@ -12147,7 +12166,7 @@
       <c r="Q66" s="4"/>
       <c r="R66" s="4"/>
     </row>
-    <row r="67" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>0</v>
       </c>
@@ -12171,7 +12190,7 @@
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
     </row>
-    <row r="68" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>2</v>
       </c>
@@ -12197,7 +12216,7 @@
       <c r="Q68" s="4"/>
       <c r="R68" s="4"/>
     </row>
-    <row r="69" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A69" s="19"/>
       <c r="B69" s="19"/>
       <c r="C69" s="20"/>
@@ -12217,7 +12236,7 @@
       <c r="Q69" s="4"/>
       <c r="R69" s="4"/>
     </row>
-    <row r="70" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="9"/>
@@ -12237,7 +12256,7 @@
       <c r="Q70" s="4"/>
       <c r="R70" s="4"/>
     </row>
-    <row r="71" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="9"/>
@@ -12257,7 +12276,7 @@
       <c r="Q71" s="4"/>
       <c r="R71" s="4"/>
     </row>
-    <row r="72" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="9"/>
@@ -12277,7 +12296,7 @@
       <c r="Q72" s="4"/>
       <c r="R72" s="4"/>
     </row>
-    <row r="73" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="9"/>
@@ -12297,7 +12316,7 @@
       <c r="Q73" s="4"/>
       <c r="R73" s="4"/>
     </row>
-    <row r="74" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="23"/>
       <c r="B74" s="23"/>
       <c r="C74" s="24"/>
@@ -12317,7 +12336,7 @@
       <c r="Q74" s="4"/>
       <c r="R74" s="4"/>
     </row>
-    <row r="75" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14" t="s">
         <v>22</v>
       </c>
@@ -12342,7 +12361,7 @@
       <c r="Q75" s="4"/>
       <c r="R75" s="4"/>
     </row>
-    <row r="76" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="16"/>
       <c r="B76" s="16"/>
       <c r="C76" s="16"/>
@@ -12362,7 +12381,7 @@
       <c r="Q76" s="4"/>
       <c r="R76" s="4"/>
     </row>
-    <row r="77" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
@@ -12386,7 +12405,7 @@
       <c r="Q77" s="4"/>
       <c r="R77" s="4"/>
     </row>
-    <row r="78" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>2</v>
       </c>
@@ -12412,7 +12431,7 @@
       <c r="Q78" s="4"/>
       <c r="R78" s="4"/>
     </row>
-    <row r="79" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A79" s="19"/>
       <c r="B79" s="19"/>
       <c r="C79" s="20"/>
@@ -12432,7 +12451,7 @@
       <c r="Q79" s="4"/>
       <c r="R79" s="4"/>
     </row>
-    <row r="80" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="9"/>
@@ -12452,7 +12471,7 @@
       <c r="Q80" s="4"/>
       <c r="R80" s="4"/>
     </row>
-    <row r="81" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="9"/>
@@ -12472,7 +12491,7 @@
       <c r="Q81" s="4"/>
       <c r="R81" s="4"/>
     </row>
-    <row r="82" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="9"/>
@@ -12492,7 +12511,7 @@
       <c r="Q82" s="4"/>
       <c r="R82" s="4"/>
     </row>
-    <row r="83" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="9"/>
@@ -12512,7 +12531,7 @@
       <c r="Q83" s="4"/>
       <c r="R83" s="4"/>
     </row>
-    <row r="84" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="9"/>
@@ -12532,7 +12551,7 @@
       <c r="Q84" s="4"/>
       <c r="R84" s="4"/>
     </row>
-    <row r="85" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="9"/>
@@ -12552,7 +12571,7 @@
       <c r="Q85" s="4"/>
       <c r="R85" s="4"/>
     </row>
-    <row r="86" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="23"/>
       <c r="B86" s="23"/>
       <c r="C86" s="24"/>
@@ -12572,7 +12591,7 @@
       <c r="Q86" s="4"/>
       <c r="R86" s="4"/>
     </row>
-    <row r="87" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="14" t="s">
         <v>22</v>
       </c>
@@ -12597,7 +12616,7 @@
       <c r="Q87" s="4"/>
       <c r="R87" s="4"/>
     </row>
-    <row r="88" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A88" s="16"/>
       <c r="B88" s="16"/>
       <c r="C88" s="16"/>
@@ -12617,7 +12636,7 @@
       <c r="Q88" s="4"/>
       <c r="R88" s="4"/>
     </row>
-    <row r="89" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A89" s="27"/>
       <c r="B89" s="27"/>
       <c r="C89" s="27"/>
@@ -12637,7 +12656,7 @@
       <c r="Q89" s="4"/>
       <c r="R89" s="4"/>
     </row>
-    <row r="90" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A90" s="27"/>
       <c r="B90" s="27"/>
       <c r="C90" s="27"/>
@@ -12657,7 +12676,7 @@
       <c r="Q90" s="4"/>
       <c r="R90" s="4"/>
     </row>
-    <row r="91" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A91" s="27"/>
       <c r="B91" s="27"/>
       <c r="C91" s="27"/>
@@ -12677,7 +12696,7 @@
       <c r="Q91" s="4"/>
       <c r="R91" s="4"/>
     </row>
-    <row r="92" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A92" s="27"/>
       <c r="B92" s="27"/>
       <c r="C92" s="27"/>
@@ -12697,7 +12716,7 @@
       <c r="Q92" s="4"/>
       <c r="R92" s="4"/>
     </row>
-    <row r="93" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A93" s="27"/>
       <c r="B93" s="27"/>
       <c r="C93" s="27"/>
@@ -12717,7 +12736,7 @@
       <c r="Q93" s="4"/>
       <c r="R93" s="4"/>
     </row>
-    <row r="94" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A94" s="27"/>
       <c r="B94" s="27"/>
       <c r="C94" s="27"/>
@@ -12737,7 +12756,7 @@
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
     </row>
-    <row r="95" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A95" s="27"/>
       <c r="B95" s="27"/>
       <c r="C95" s="27"/>
@@ -12757,7 +12776,7 @@
       <c r="Q95" s="4"/>
       <c r="R95" s="4"/>
     </row>
-    <row r="96" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A96" s="27"/>
       <c r="B96" s="27"/>
       <c r="C96" s="27"/>
@@ -12777,7 +12796,7 @@
       <c r="Q96" s="4"/>
       <c r="R96" s="4"/>
     </row>
-    <row r="97" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A97" s="27"/>
       <c r="B97" s="27"/>
       <c r="C97" s="27"/>
@@ -12797,7 +12816,7 @@
       <c r="Q97" s="4"/>
       <c r="R97" s="4"/>
     </row>
-    <row r="98" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A98" s="27"/>
       <c r="B98" s="27"/>
       <c r="C98" s="27"/>
@@ -12817,7 +12836,7 @@
       <c r="Q98" s="4"/>
       <c r="R98" s="4"/>
     </row>
-    <row r="99" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A99" s="27"/>
       <c r="B99" s="27"/>
       <c r="C99" s="27"/>
@@ -12837,7 +12856,7 @@
       <c r="Q99" s="4"/>
       <c r="R99" s="4"/>
     </row>
-    <row r="100" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:18" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A100" s="28"/>
       <c r="B100" s="28"/>
       <c r="C100" s="28"/>
@@ -12874,19 +12893,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04752183-13CB-498C-B47A-4401EA9BDEF9}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12896,7 +12915,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -12910,7 +12929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="54" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>249</v>
       </c>
@@ -12923,8 +12942,10 @@
       <c r="D3" s="47" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="54" x14ac:dyDescent="0.25">
+      <c r="H3" s="77"/>
+      <c r="I3" s="78"/>
+    </row>
+    <row r="4" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>254</v>
       </c>
@@ -12937,8 +12958,10 @@
       <c r="D4" s="51" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="H4" s="77"/>
+      <c r="I4" s="78"/>
+    </row>
+    <row r="5" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>253</v>
       </c>
@@ -12951,8 +12974,9 @@
       <c r="D5" s="51" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="H5" s="77"/>
+    </row>
+    <row r="6" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>259</v>
       </c>
@@ -12965,89 +12989,94 @@
       <c r="D6" s="51" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H6" s="77"/>
+      <c r="I6" s="78"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="B7" s="69">
+      <c r="B7" s="71">
         <v>6</v>
       </c>
-      <c r="C7" s="66">
+      <c r="C7" s="68">
         <v>43977</v>
       </c>
-      <c r="D7" s="72" t="s">
+      <c r="D7" s="74" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H7" s="77"/>
+      <c r="I7" s="78"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>261</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="73"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="72"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="75"/>
+      <c r="F8" s="78"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>262</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="73"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="72"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="75"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="53" t="s">
         <v>263</v>
       </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="73"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="72"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="75"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>264</v>
       </c>
-      <c r="B11" s="70"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="73"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="72"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="75"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>265</v>
       </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="73"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="72"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="75"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="62" t="s">
         <v>266</v>
       </c>
-      <c r="B13" s="70"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="73"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="72"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="75"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="62" t="s">
         <v>267</v>
       </c>
-      <c r="B14" s="71"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="74"/>
-    </row>
-    <row r="15" spans="1:4" ht="27" x14ac:dyDescent="0.25">
+      <c r="B14" s="73"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="76"/>
+    </row>
+    <row r="15" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
         <v>256</v>
       </c>
       <c r="B15" s="53">
         <v>1</v>
       </c>
-      <c r="C15" s="68"/>
+      <c r="C15" s="70"/>
       <c r="D15" s="54"/>
     </row>
-    <row r="16" spans="1:4" ht="27" x14ac:dyDescent="0.25">
-      <c r="A16" s="69" t="s">
+    <row r="16" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="71" t="s">
         <v>257</v>
       </c>
       <c r="B16" s="63">
@@ -13061,43 +13090,51 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="70"/>
-      <c r="B17" s="53">
+      <c r="A17" s="72"/>
+      <c r="B17" s="66">
         <v>4</v>
       </c>
       <c r="C17" s="64">
         <v>43979</v>
       </c>
-      <c r="D17" s="54"/>
-    </row>
-    <row r="18" spans="1:4" ht="27" x14ac:dyDescent="0.25">
-      <c r="A18" s="70"/>
-      <c r="B18" s="53">
+      <c r="D17" s="79" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="72"/>
+      <c r="B18" s="66">
         <v>4</v>
       </c>
       <c r="C18" s="64">
         <v>43980</v>
       </c>
-      <c r="D18" s="54" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
-      <c r="B19" s="53"/>
+      <c r="D18" s="80"/>
+    </row>
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A19" s="72"/>
+      <c r="B19" s="66">
+        <v>4</v>
+      </c>
       <c r="C19" s="64">
         <v>43982</v>
       </c>
-      <c r="D19" s="54"/>
-    </row>
-    <row r="20" spans="1:4" ht="27" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="53"/>
+      <c r="D19" s="54" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="66" x14ac:dyDescent="0.25">
+      <c r="A20" s="67" t="s">
+        <v>235</v>
+      </c>
+      <c r="B20" s="63">
+        <v>1.5</v>
+      </c>
       <c r="C20" s="64">
-        <v>43982</v>
+        <v>43983</v>
       </c>
       <c r="D20" s="54" t="s">
-        <v>270</v>
+        <v>316</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -13136,36 +13173,36 @@
       <c r="C26" s="54"/>
       <c r="D26" s="54"/>
     </row>
-    <row r="27" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="55"/>
       <c r="B27" s="55"/>
       <c r="C27" s="56"/>
       <c r="D27" s="56"/>
     </row>
-    <row r="28" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="53"/>
       <c r="B28" s="53"/>
       <c r="C28" s="54"/>
       <c r="D28" s="54"/>
     </row>
-    <row r="29" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B29" s="14">
         <f>SUM(B3:B27)</f>
-        <v>30.5</v>
+        <v>36</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
     </row>
-    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="16"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
       <c r="D30" s="16"/>
     </row>
-    <row r="31" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -13175,7 +13212,7 @@
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
@@ -13247,13 +13284,13 @@
       <c r="C42" s="26"/>
       <c r="D42" s="26"/>
     </row>
-    <row r="43" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="23"/>
       <c r="B43" s="23"/>
       <c r="C43" s="24"/>
       <c r="D43" s="24"/>
     </row>
-    <row r="44" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
         <v>22</v>
       </c>
@@ -13264,13 +13301,13 @@
       <c r="C44" s="15"/>
       <c r="D44" s="15"/>
     </row>
-    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
       <c r="D45" s="16"/>
     </row>
-    <row r="46" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -13280,7 +13317,7 @@
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>2</v>
       </c>
@@ -13322,13 +13359,13 @@
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
     </row>
-    <row r="53" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="23"/>
       <c r="B53" s="23"/>
       <c r="C53" s="24"/>
       <c r="D53" s="24"/>
     </row>
-    <row r="54" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="14" t="s">
         <v>22</v>
       </c>
@@ -13339,13 +13376,13 @@
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
     </row>
-    <row r="55" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="16"/>
       <c r="B55" s="16"/>
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
     </row>
-    <row r="56" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
@@ -13355,7 +13392,7 @@
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>2</v>
       </c>
@@ -13409,13 +13446,13 @@
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
     </row>
-    <row r="65" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="23"/>
       <c r="B65" s="23"/>
       <c r="C65" s="24"/>
       <c r="D65" s="24"/>
     </row>
-    <row r="66" spans="1:4" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="14" t="s">
         <v>22</v>
       </c>
@@ -13426,18 +13463,19 @@
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
     </row>
-    <row r="67" spans="1:4" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A67" s="16"/>
       <c r="B67" s="16"/>
       <c r="C67" s="16"/>
       <c r="D67" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C7:C15"/>
     <mergeCell ref="B7:B14"/>
     <mergeCell ref="D7:D14"/>
     <mergeCell ref="A16:A19"/>
+    <mergeCell ref="D17:D18"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B29 B44 B54 B66" xr:uid="{DA0CB379-8208-4014-8C0C-0521765B9A4F}">

</xml_diff>

<commit_message>
Journal HM + new DB
</commit_message>
<xml_diff>
--- a/LM_Journal_Travail_V1.0.xlsx
+++ b/LM_Journal_Travail_V1.0.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projet\Love-Mirroring\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCF1AF1-E35B-4A2C-9DE8-056B5A596CB4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Equipe" sheetId="1" r:id="rId1"/>
@@ -30,7 +24,7 @@
     <definedName name="NBLecons">#REF!</definedName>
     <definedName name="TachesPlanifiees">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -45,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="350">
   <si>
     <t>Jalon</t>
   </si>
@@ -1150,11 +1144,21 @@
   <si>
     <t>Le chat bot est enfin connecté et je peux envoyer des messages et le recevoir depuis le bot. Je vais maintenant configurer les commandes.</t>
   </si>
+  <si>
+    <t>Faire fonctionner le projet à l'ES
+Modification de la base données opour pouvoir Ignorer un utilisateur OK
+Mise à jour de la base de donnée pour savoir si le compte viens de facebook Ok
+Change de la recherche Admin pour les utilisateurs non Facebook seulement
+Changement l'ors d'un like l'utilisateur liker n'est pas ignorer par défaut</t>
+  </si>
+  <si>
+    <t>User/Admin/DB</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
     <numFmt numFmtId="165" formatCode="dd\.mm\.yy"/>
@@ -1926,7 +1930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -4923,10 +4927,10 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B73:B80 B16:B31 B36:B37 B39:B43 B3:B8 B63:B68 B10:B11 B48:B58" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B73:B80 B16:B31 B36:B37 B39:B43 B3:B8 B63:B68 B10:B11 B48:B58">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B12 B32 B44 B59 B69 B81" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B12 B32 B44 B59 B69 B81">
       <formula1>0</formula1>
       <formula2>DureePeriode-1</formula2>
     </dataValidation>
@@ -4937,10 +4941,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB7A04D-A66F-4A89-83F1-9B353075A776}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
@@ -7759,11 +7763,11 @@
     </row>
   </sheetData>
   <dataValidations xWindow="188" yWindow="522" count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B12 B34 B56 B98 B86 B76 G76" xr:uid="{41F29EDA-D509-4469-8DFB-6A4CE4CEAE07}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B12 B34 B56 B98 B86 B76 G76">
       <formula1>0</formula1>
       <formula2>DureePeriode-1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B90:B97 B38:B39 B41:B45 B80:B85 B10:B11 B3:B8 B16:B33 B60:B76" xr:uid="{3039B7E3-952E-4B34-B612-E5A0C049619C}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B90:B97 B38:B39 B41:B45 B80:B85 B10:B11 B3:B8 B16:B33 B60:B76">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -7773,7 +7777,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{716E2DDB-6361-470B-ACF3-8FDF9046203A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R113"/>
   <sheetViews>
     <sheetView topLeftCell="A92" workbookViewId="0">
@@ -10552,10 +10556,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B92:B99 B17:B38 B71:B87 B46:B66 B3:B8 B10:B12 B43:B44" xr:uid="{76F8C2A5-22FC-42B6-BF5F-FD1899EE52B8}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B92:B99 B17:B38 B71:B87 B46:B66 B3:B8 B10:B12 B43:B44">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B13 B39 B67 B100 B88" xr:uid="{BD151BE4-B931-4CBD-823B-9C753DC07C8D}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B13 B39 B67 B100 B88">
       <formula1>0</formula1>
       <formula2>DureePeriode-1</formula2>
     </dataValidation>
@@ -10565,11 +10569,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F222774-5003-490D-9078-78D1F6F89A4A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R100"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -12375,11 +12379,19 @@
       <c r="Q68" s="4"/>
       <c r="R68" s="4"/>
     </row>
-    <row r="69" spans="1:18" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="A69" s="19"/>
-      <c r="B69" s="19"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
+    <row r="69" spans="1:18" ht="67.5" x14ac:dyDescent="0.3">
+      <c r="A69" s="19" t="s">
+        <v>349</v>
+      </c>
+      <c r="B69" s="19">
+        <v>5</v>
+      </c>
+      <c r="C69" s="57">
+        <v>43990</v>
+      </c>
+      <c r="D69" s="20" t="s">
+        <v>348</v>
+      </c>
       <c r="E69" s="10"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -12501,7 +12513,7 @@
       </c>
       <c r="B75" s="14">
         <f>SUM(B69:B74)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C75" s="15"/>
       <c r="D75" s="15"/>
@@ -13037,10 +13049,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B79:B86 B10:B13 B38:B39 B18:B33 B41:B49 B69:B74 B3:B8 B54:B64" xr:uid="{64471589-AB55-4AF0-A3CB-2C4DA302E1FD}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B79:B86 B10:B13 B38:B39 B18:B33 B41:B49 B69:B74 B3:B8 B54:B64">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B87 B34 B50 B65 B75 B14" xr:uid="{E5C4B3DD-C4A0-4BDF-8596-69EE95FDEE2C}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B87 B34 B50 B65 B75 B14">
       <formula1>0</formula1>
       <formula2>DureePeriode-1</formula2>
     </dataValidation>
@@ -13051,7 +13063,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04752183-13CB-498C-B47A-4401EA9BDEF9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -13637,11 +13649,11 @@
     <mergeCell ref="D17:D18"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B29 B44 B54 B66" xr:uid="{DA0CB379-8208-4014-8C0C-0521765B9A4F}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" prompt="Dépassement de durée - Le nombre de minutes introduites dépasse la durée d'une période. Veuillez confirmer ... Le calcul du total sera juste dans tous les cas._x000a_" sqref="B29 B44 B54 B66">
       <formula1>0</formula1>
       <formula2>DureePeriode-1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B58:B65 B33:B43 B48:B53 B3:B4 B6:B7 B15:B28" xr:uid="{FBF1D711-E5DD-4569-8B54-987F2C077F7C}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" prompt="Durée en 1/3 de période - Le nombre doit être de type entier" sqref="B58:B65 B33:B43 B48:B53 B3:B4 B6:B7 B15:B28">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>